<commit_message>
Calculo de média e desvio padrão finalizado
</commit_message>
<xml_diff>
--- a/ReconciliationReport.xlsx
+++ b/ReconciliationReport.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="TimeDistanceReport" r:id="rId3" sheetId="1"/>
+    <sheet name="Statistics" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>t1</t>
   </si>
@@ -126,6 +127,21 @@
   </si>
   <si>
     <t>dTOTAL</t>
+  </si>
+  <si>
+    <t>Médias</t>
+  </si>
+  <si>
+    <t>Desvio Padrão</t>
+  </si>
+  <si>
+    <t>Polarização (bias)</t>
+  </si>
+  <si>
+    <t>Precisão</t>
+  </si>
+  <si>
+    <t>Incerteza</t>
   </si>
 </sst>
 </file>
@@ -294,1162 +310,1567 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.631E12</v>
+        <v>17.898909</v>
       </c>
       <c r="B2" t="n">
-        <v>145.81548102229092</v>
+        <v>149.93845820171066</v>
       </c>
       <c r="C2" t="n">
-        <v>5.97E11</v>
+        <v>3.757486</v>
       </c>
       <c r="D2" t="n">
-        <v>49.63374177097822</v>
+        <v>49.63186634021935</v>
       </c>
       <c r="E2" t="n">
-        <v>4.336E12</v>
+        <v>35.755863999999995</v>
       </c>
       <c r="F2" t="n">
-        <v>303.2012931032043</v>
+        <v>299.8174014579871</v>
       </c>
       <c r="G2" t="n">
-        <v>1.146E12</v>
+        <v>9.488608</v>
       </c>
       <c r="H2" t="n">
-        <v>34.67924960995788</v>
+        <v>33.921618527877285</v>
       </c>
       <c r="I2" t="n">
-        <v>1.869E12</v>
+        <v>15.747050999999999</v>
       </c>
       <c r="J2" t="n">
-        <v>123.14939961042103</v>
+        <v>123.14939961042148</v>
       </c>
       <c r="K2" t="n">
-        <v>1.426E12</v>
+        <v>11.758607</v>
       </c>
       <c r="L2" t="n">
-        <v>103.00859782254975</v>
+        <v>103.0085978093997</v>
       </c>
       <c r="M2" t="n">
-        <v>1.454E12</v>
+        <v>11.392631</v>
       </c>
       <c r="N2" t="n">
-        <v>98.56426092704851</v>
+        <v>98.5642540924681</v>
       </c>
       <c r="O2" t="n">
-        <v>2.25E11</v>
+        <v>1.6427029999999998</v>
       </c>
       <c r="P2" t="n">
-        <v>14.426896677450259</v>
+        <v>12.366105742049172</v>
       </c>
       <c r="Q2" t="n">
-        <v>2.163E12</v>
+        <v>16.624617</v>
       </c>
       <c r="R2" t="n">
-        <v>144.14075436299777</v>
+        <v>144.1400009658363</v>
       </c>
       <c r="S2" t="n">
-        <v>4.36E11</v>
+        <v>3.2252009999999998</v>
       </c>
       <c r="T2" t="n">
-        <v>30.402374312591405</v>
+        <v>30.402900287919238</v>
       </c>
       <c r="U2" t="n">
-        <v>3.824E12</v>
+        <v>30.479109</v>
       </c>
       <c r="V2" t="n">
-        <v>177.6468874907705</v>
+        <v>178.81405575630765</v>
       </c>
       <c r="W2" t="n">
-        <v>1.81E11</v>
+        <v>1.0946909999999999</v>
       </c>
       <c r="X2" t="n">
-        <v>7.8786144895925645</v>
+        <v>7.308795522299533</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.841E12</v>
+        <v>13.197495</v>
       </c>
       <c r="Z2" t="n">
-        <v>106.20856441042838</v>
+        <v>106.17384432256358</v>
       </c>
       <c r="AA2" t="n">
-        <v>2.512E12</v>
+        <v>16.972752</v>
       </c>
       <c r="AB2" t="n">
-        <v>146.56558737304977</v>
+        <v>148.62657551991197</v>
       </c>
       <c r="AC2" t="n">
-        <v>1.204E12</v>
+        <v>7.971165999999999</v>
       </c>
       <c r="AD2" t="n">
-        <v>68.07257850341443</v>
+        <v>68.07280354279715</v>
       </c>
       <c r="AE2" t="n">
-        <v>1.814E12</v>
+        <v>12.383906</v>
       </c>
       <c r="AF2" t="n">
-        <v>73.88080507054315</v>
+        <v>72.78890419032814</v>
       </c>
       <c r="AG2" t="n">
-        <v>2.482E12</v>
+        <v>16.169334</v>
       </c>
       <c r="AH2" t="n">
-        <v>115.62701977630809</v>
+        <v>115.62734605898436</v>
       </c>
       <c r="AI2" t="n">
-        <v>2.663E12</v>
+        <v>16.930766</v>
       </c>
       <c r="AJ2" t="n">
-        <v>95.1878964172281</v>
+        <v>95.0182142411004</v>
       </c>
       <c r="AK2" t="n">
-        <v>3.2804E13</v>
+        <v>242.49089600000002</v>
       </c>
       <c r="AL2" t="n">
-        <v>1838.090002750825</v>
+        <v>1837.371142190181</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5.97E11</v>
+        <v>28.474777</v>
       </c>
       <c r="B3" t="n">
-        <v>49.63374177097822</v>
+        <v>144.79113232676042</v>
       </c>
       <c r="C3" t="n">
-        <v>1.146E12</v>
+        <v>6.347958</v>
       </c>
       <c r="D3" t="n">
-        <v>34.67924960995788</v>
+        <v>49.4281421382434</v>
       </c>
       <c r="E3" t="n">
-        <v>1.426E12</v>
+        <v>47.675554999999996</v>
       </c>
       <c r="F3" t="n">
-        <v>103.00859782254975</v>
+        <v>303.9743034288899</v>
       </c>
       <c r="G3" t="n">
-        <v>2.25E11</v>
+        <v>33.443861</v>
       </c>
       <c r="H3" t="n">
-        <v>14.426896677450259</v>
+        <v>34.19351301809343</v>
       </c>
       <c r="I3" t="n">
-        <v>4.36E11</v>
+        <v>24.469026</v>
       </c>
       <c r="J3" t="n">
-        <v>30.402374312591405</v>
+        <v>122.99571421928556</v>
       </c>
       <c r="K3" t="n">
-        <v>1.81E11</v>
+        <v>15.750368</v>
       </c>
       <c r="L3" t="n">
-        <v>7.8786144895925645</v>
+        <v>103.94788935803092</v>
       </c>
       <c r="M3" t="n">
-        <v>2.512E12</v>
+        <v>14.519493</v>
       </c>
       <c r="N3" t="n">
-        <v>146.56558737304977</v>
+        <v>99.97635003241408</v>
       </c>
       <c r="O3" t="n">
-        <v>1.814E12</v>
+        <v>2.1509359999999997</v>
       </c>
       <c r="P3" t="n">
-        <v>73.88080507054315</v>
+        <v>12.769546349331335</v>
       </c>
       <c r="Q3" t="n">
-        <v>2.663E12</v>
+        <v>21.478212</v>
       </c>
       <c r="R3" t="n">
-        <v>95.1878964172281</v>
+        <v>143.99615177300814</v>
       </c>
       <c r="S3" t="n">
-        <v>4.541E12</v>
+        <v>4.267454</v>
       </c>
       <c r="T3" t="n">
-        <v>144.82315115315194</v>
+        <v>30.846957897213883</v>
       </c>
       <c r="U3" t="n">
-        <v>7.632E12</v>
+        <v>26.427544</v>
       </c>
       <c r="V3" t="n">
-        <v>303.94500766324705</v>
+        <v>178.77194410944162</v>
       </c>
       <c r="W3" t="n">
-        <v>3.981E12</v>
+        <v>1.290508</v>
       </c>
       <c r="X3" t="n">
-        <v>122.9957142192859</v>
+        <v>7.2994120601485974</v>
       </c>
       <c r="Y3" t="n">
-        <v>2.447E12</v>
+        <v>15.445687999999999</v>
       </c>
       <c r="Z3" t="n">
-        <v>99.97635003241408</v>
+        <v>106.19326311778377</v>
       </c>
       <c r="AA3" t="n">
-        <v>3.579E12</v>
+        <v>21.827087999999996</v>
       </c>
       <c r="AB3" t="n">
-        <v>143.9961520779833</v>
+        <v>144.36096860648854</v>
       </c>
       <c r="AC3" t="n">
-        <v>4.491E12</v>
+        <v>10.471074</v>
       </c>
       <c r="AD3" t="n">
-        <v>178.7719518253857</v>
+        <v>71.20918678179419</v>
       </c>
       <c r="AE3" t="n">
-        <v>2.708E12</v>
+        <v>16.423234</v>
       </c>
       <c r="AF3" t="n">
-        <v>106.19326311778377</v>
+        <v>73.09112240986315</v>
       </c>
       <c r="AG3" t="n">
-        <v>1.818E12</v>
+        <v>19.306097</v>
       </c>
       <c r="AH3" t="n">
-        <v>69.38555967837692</v>
+        <v>115.20492014937258</v>
       </c>
       <c r="AI3" t="n">
-        <v>3.417E12</v>
+        <v>20.399605</v>
       </c>
       <c r="AJ3" t="n">
-        <v>115.20492014937258</v>
+        <v>93.98100613501015</v>
       </c>
       <c r="AK3" t="n">
-        <v>4.5614E13</v>
+        <v>330.168478</v>
       </c>
       <c r="AL3" t="n">
-        <v>1840.9558334609421</v>
+        <v>1837.0315239111737</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4.336E12</v>
+        <v>30.74215</v>
       </c>
       <c r="B4" t="n">
-        <v>303.2012931032043</v>
+        <v>144.76342178633664</v>
       </c>
       <c r="C4" t="n">
-        <v>1.426E12</v>
+        <v>7.466755999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>103.00859782254975</v>
+        <v>49.28402626464489</v>
       </c>
       <c r="E4" t="n">
-        <v>2.163E12</v>
+        <v>49.92704</v>
       </c>
       <c r="F4" t="n">
-        <v>144.14075436299777</v>
+        <v>304.36899839708315</v>
       </c>
       <c r="G4" t="n">
-        <v>1.81E11</v>
+        <v>12.573599999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>7.8786144895925645</v>
+        <v>35.217562032325645</v>
       </c>
       <c r="I4" t="n">
-        <v>1.204E12</v>
+        <v>19.182675999999997</v>
       </c>
       <c r="J4" t="n">
-        <v>68.07257850341443</v>
+        <v>121.52439643674268</v>
       </c>
       <c r="K4" t="n">
-        <v>2.663E12</v>
+        <v>14.613634999999999</v>
       </c>
       <c r="L4" t="n">
-        <v>95.1878964172281</v>
+        <v>104.08029712859968</v>
       </c>
       <c r="M4" t="n">
-        <v>1.111E12</v>
+        <v>14.147934999999999</v>
       </c>
       <c r="N4" t="n">
-        <v>49.42828140479463</v>
+        <v>99.82816265519148</v>
       </c>
       <c r="O4" t="n">
-        <v>3.981E12</v>
+        <v>1.771649</v>
       </c>
       <c r="P4" t="n">
-        <v>122.9957142192859</v>
+        <v>11.786607227173363</v>
       </c>
       <c r="Q4" t="n">
-        <v>3.6E11</v>
+        <v>20.027079999999998</v>
       </c>
       <c r="R4" t="n">
-        <v>12.769546349331335</v>
+        <v>145.24798293202514</v>
       </c>
       <c r="S4" t="n">
-        <v>4.491E12</v>
+        <v>3.9648689999999993</v>
       </c>
       <c r="T4" t="n">
-        <v>178.7719518253857</v>
+        <v>31.055146976152514</v>
       </c>
       <c r="U4" t="n">
-        <v>3.804E12</v>
+        <v>24.320154</v>
       </c>
       <c r="V4" t="n">
-        <v>146.1846019184518</v>
+        <v>177.89660500343757</v>
       </c>
       <c r="W4" t="n">
-        <v>3.417E12</v>
+        <v>1.046655</v>
       </c>
       <c r="X4" t="n">
-        <v>115.20492014937258</v>
+        <v>7.859939908723845</v>
       </c>
       <c r="Y4" t="n">
-        <v>5.334E12</v>
+        <v>14.420541</v>
       </c>
       <c r="Z4" t="n">
-        <v>144.80210506486105</v>
+        <v>104.50123124782431</v>
       </c>
       <c r="AA4" t="n">
-        <v>2.31E12</v>
+        <v>19.811963</v>
       </c>
       <c r="AB4" t="n">
-        <v>35.522378857788624</v>
+        <v>147.5772135289974</v>
       </c>
       <c r="AC4" t="n">
-        <v>2.494E12</v>
+        <v>9.506752</v>
       </c>
       <c r="AD4" t="n">
-        <v>99.82806549513418</v>
+        <v>68.81902771475166</v>
       </c>
       <c r="AE4" t="n">
-        <v>6.76E11</v>
+        <v>14.099295000000001</v>
       </c>
       <c r="AF4" t="n">
-        <v>29.138155252555293</v>
+        <v>73.34549737204657</v>
       </c>
       <c r="AG4" t="n">
-        <v>2.594E12</v>
+        <v>17.889508</v>
       </c>
       <c r="AH4" t="n">
-        <v>106.46633883299887</v>
+        <v>114.4412242097219</v>
       </c>
       <c r="AI4" t="n">
-        <v>2.47E12</v>
+        <v>25.458251999999998</v>
       </c>
       <c r="AJ4" t="n">
-        <v>72.94929513009538</v>
+        <v>96.54324127822156</v>
       </c>
       <c r="AK4" t="n">
-        <v>4.5015E13</v>
+        <v>300.97050999999993</v>
       </c>
       <c r="AL4" t="n">
-        <v>1835.5510891990423</v>
+        <v>1838.1405820999998</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.146E12</v>
+        <v>29.715474</v>
       </c>
       <c r="B5" t="n">
-        <v>34.67924960995788</v>
+        <v>145.2707825212945</v>
       </c>
       <c r="C5" t="n">
-        <v>2.25E11</v>
+        <v>6.144475999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>14.426896677450259</v>
+        <v>48.587830605834</v>
       </c>
       <c r="E5" t="n">
-        <v>1.81E11</v>
+        <v>44.063660999999996</v>
       </c>
       <c r="F5" t="n">
-        <v>7.8786144895925645</v>
+        <v>305.0251470345246</v>
       </c>
       <c r="G5" t="n">
-        <v>1.814E12</v>
+        <v>11.993674</v>
       </c>
       <c r="H5" t="n">
-        <v>73.88080507054315</v>
+        <v>34.3771325501321</v>
       </c>
       <c r="I5" t="n">
-        <v>4.541E12</v>
+        <v>18.010492</v>
       </c>
       <c r="J5" t="n">
-        <v>144.82315115315194</v>
+        <v>120.89671360334557</v>
       </c>
       <c r="K5" t="n">
-        <v>3.981E12</v>
+        <v>13.314100999999999</v>
       </c>
       <c r="L5" t="n">
-        <v>122.9957142192859</v>
+        <v>105.21534067161406</v>
       </c>
       <c r="M5" t="n">
-        <v>3.579E12</v>
+        <v>13.389275000000001</v>
       </c>
       <c r="N5" t="n">
-        <v>143.9961520779833</v>
+        <v>100.68274205387138</v>
       </c>
       <c r="O5" t="n">
-        <v>2.708E12</v>
+        <v>1.521847</v>
       </c>
       <c r="P5" t="n">
-        <v>106.19326311778377</v>
+        <v>10.524091602296494</v>
       </c>
       <c r="Q5" t="n">
-        <v>3.417E12</v>
+        <v>18.39313</v>
       </c>
       <c r="R5" t="n">
-        <v>115.20492014937258</v>
+        <v>145.12451763179752</v>
       </c>
       <c r="S5" t="n">
-        <v>1.176E12</v>
+        <v>3.7781329999999995</v>
       </c>
       <c r="T5" t="n">
-        <v>49.2842043518537</v>
+        <v>31.013559215837176</v>
       </c>
       <c r="U5" t="n">
-        <v>2.629E12</v>
+        <v>42.347043</v>
       </c>
       <c r="V5" t="n">
-        <v>104.08026361686245</v>
+        <v>177.83228794072056</v>
       </c>
       <c r="W5" t="n">
-        <v>6.76E11</v>
+        <v>1.364185</v>
       </c>
       <c r="X5" t="n">
-        <v>29.138155252555293</v>
+        <v>7.153941978695684</v>
       </c>
       <c r="Y5" t="n">
-        <v>3.516E12</v>
+        <v>15.296091999999998</v>
       </c>
       <c r="Z5" t="n">
-        <v>147.57665066617392</v>
+        <v>106.90803706588235</v>
       </c>
       <c r="AA5" t="n">
-        <v>3.844E12</v>
+        <v>19.524008</v>
       </c>
       <c r="AB5" t="n">
-        <v>96.58803754419569</v>
+        <v>147.59389558046132</v>
       </c>
       <c r="AC5" t="n">
-        <v>7.947E12</v>
+        <v>8.831647</v>
       </c>
       <c r="AD5" t="n">
-        <v>305.0251841267425</v>
+        <v>67.42423043569806</v>
       </c>
       <c r="AE5" t="n">
-        <v>2.254E12</v>
+        <v>14.424760000000001</v>
       </c>
       <c r="AF5" t="n">
-        <v>100.6827400343019</v>
+        <v>74.06952057917806</v>
       </c>
       <c r="AG5" t="n">
-        <v>7.777E12</v>
+        <v>18.677448</v>
       </c>
       <c r="AH5" t="n">
-        <v>177.8329152918277</v>
+        <v>114.72797460170068</v>
       </c>
       <c r="AI5" t="n">
-        <v>1.541E12</v>
+        <v>33.829932</v>
       </c>
       <c r="AJ5" t="n">
-        <v>67.42423043569806</v>
+        <v>95.16207850854903</v>
       </c>
       <c r="AK5" t="n">
-        <v>5.2952E13</v>
+        <v>314.619378</v>
       </c>
       <c r="AL5" t="n">
-        <v>1841.7111478853326</v>
+        <v>1837.5898241814332</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1.869E12</v>
+        <v>30.770184999999998</v>
       </c>
       <c r="B6" t="n">
-        <v>123.14939961042103</v>
+        <v>146.08054717074904</v>
       </c>
       <c r="C6" t="n">
-        <v>4.36E11</v>
+        <v>6.623729999999999</v>
       </c>
       <c r="D6" t="n">
-        <v>30.402374312591405</v>
+        <v>48.24785877040364</v>
       </c>
       <c r="E6" t="n">
-        <v>1.204E12</v>
+        <v>47.622342999999994</v>
       </c>
       <c r="F6" t="n">
-        <v>68.07257850341443</v>
+        <v>304.14924379680895</v>
       </c>
       <c r="G6" t="n">
-        <v>4.541E12</v>
+        <v>26.39798</v>
       </c>
       <c r="H6" t="n">
-        <v>144.82315115315194</v>
+        <v>33.88436077250657</v>
       </c>
       <c r="I6" t="n">
-        <v>2.698E12</v>
+        <v>24.963516</v>
       </c>
       <c r="J6" t="n">
-        <v>103.9478893580308</v>
+        <v>122.33658212311582</v>
       </c>
       <c r="K6" t="n">
-        <v>4.491E12</v>
+        <v>13.868027000000001</v>
       </c>
       <c r="L6" t="n">
-        <v>178.7719518253857</v>
+        <v>104.12777387555354</v>
       </c>
       <c r="M6" t="n">
-        <v>2.876E12</v>
+        <v>13.625786999999999</v>
       </c>
       <c r="N6" t="n">
-        <v>73.10663461743934</v>
+        <v>99.79811158717825</v>
       </c>
       <c r="O6" t="n">
-        <v>1.176E12</v>
+        <v>2.0435</v>
       </c>
       <c r="P6" t="n">
-        <v>49.2842043518537</v>
+        <v>14.022211181587295</v>
       </c>
       <c r="Q6" t="n">
-        <v>2.494E12</v>
+        <v>19.597824</v>
       </c>
       <c r="R6" t="n">
-        <v>99.82806549513418</v>
+        <v>144.105085300856</v>
       </c>
       <c r="S6" t="n">
-        <v>2.01E11</v>
+        <v>3.753393</v>
       </c>
       <c r="T6" t="n">
-        <v>7.8608007431755595</v>
+        <v>29.639376459193727</v>
       </c>
       <c r="U6" t="n">
-        <v>3.163E12</v>
+        <v>24.513741</v>
       </c>
       <c r="V6" t="n">
-        <v>114.44375990632011</v>
+        <v>176.0101840564164</v>
       </c>
       <c r="W6" t="n">
-        <v>7.947E12</v>
+        <v>1.289383</v>
       </c>
       <c r="X6" t="n">
-        <v>305.0251841267425</v>
+        <v>10.011508480810562</v>
       </c>
       <c r="Y6" t="n">
-        <v>2.98E11</v>
+        <v>14.889490999999998</v>
       </c>
       <c r="Z6" t="n">
-        <v>12.62901517231478</v>
+        <v>106.55160020644485</v>
       </c>
       <c r="AA6" t="n">
-        <v>2.585E12</v>
+        <v>20.437717</v>
       </c>
       <c r="AB6" t="n">
-        <v>106.90803706588281</v>
+        <v>146.4719757358821</v>
       </c>
       <c r="AC6" t="n">
-        <v>5.893E12</v>
+        <v>9.612361</v>
       </c>
       <c r="AD6" t="n">
-        <v>95.1620785085488</v>
+        <v>68.17021737359369</v>
       </c>
       <c r="AE6" t="n">
-        <v>2.65E12</v>
+        <v>15.071149</v>
       </c>
       <c r="AF6" t="n">
-        <v>33.94666829474971</v>
+        <v>73.60030166074353</v>
       </c>
       <c r="AG6" t="n">
-        <v>3.512E12</v>
+        <v>19.562092</v>
       </c>
       <c r="AH6" t="n">
-        <v>144.1051121232964</v>
+        <v>115.88756364210258</v>
       </c>
       <c r="AI6" t="n">
-        <v>3.638E12</v>
+        <v>19.049031</v>
       </c>
       <c r="AJ6" t="n">
-        <v>146.47194732482444</v>
+        <v>95.19727616159639</v>
       </c>
       <c r="AK6" t="n">
-        <v>5.1672E13</v>
+        <v>313.69124999999997</v>
       </c>
       <c r="AL6" t="n">
-        <v>1837.9388524932776</v>
+        <v>1838.291778355543</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1.426E12</v>
+        <v>36.14756</v>
       </c>
       <c r="B7" t="n">
-        <v>103.00859782254975</v>
+        <v>144.54401656910125</v>
       </c>
       <c r="C7" t="n">
-        <v>1.81E11</v>
+        <v>9.019302999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>7.8786144895925645</v>
+        <v>49.117846351323465</v>
       </c>
       <c r="E7" t="n">
-        <v>2.663E12</v>
+        <v>57.178433</v>
       </c>
       <c r="F7" t="n">
-        <v>95.1878964172281</v>
+        <v>304.831761798479</v>
       </c>
       <c r="G7" t="n">
-        <v>3.981E12</v>
+        <v>13.788754</v>
       </c>
       <c r="H7" t="n">
-        <v>122.9957142192859</v>
+        <v>34.11997998783323</v>
       </c>
       <c r="I7" t="n">
-        <v>4.491E12</v>
+        <v>21.546715</v>
       </c>
       <c r="J7" t="n">
-        <v>178.7719518253857</v>
+        <v>122.08259239318897</v>
       </c>
       <c r="K7" t="n">
-        <v>3.417E12</v>
+        <v>17.900951</v>
       </c>
       <c r="L7" t="n">
-        <v>115.20492014937258</v>
+        <v>103.36647569193963</v>
       </c>
       <c r="M7" t="n">
-        <v>2.31E12</v>
+        <v>16.992866</v>
       </c>
       <c r="N7" t="n">
-        <v>35.522378857788624</v>
+        <v>98.19493201710588</v>
       </c>
       <c r="O7" t="n">
-        <v>6.76E11</v>
+        <v>2.5347839999999997</v>
       </c>
       <c r="P7" t="n">
-        <v>29.138155252555293</v>
+        <v>16.15901133661771</v>
       </c>
       <c r="Q7" t="n">
-        <v>2.47E12</v>
+        <v>23.873815999999998</v>
       </c>
       <c r="R7" t="n">
-        <v>72.94929513009538</v>
+        <v>143.67219666490837</v>
       </c>
       <c r="S7" t="n">
-        <v>7.947E12</v>
+        <v>4.492932</v>
       </c>
       <c r="T7" t="n">
-        <v>305.0251841267425</v>
+        <v>29.276797797005884</v>
       </c>
       <c r="U7" t="n">
-        <v>3.288E12</v>
+        <v>30.550725</v>
       </c>
       <c r="V7" t="n">
-        <v>143.02002563246845</v>
+        <v>179.6359884352437</v>
       </c>
       <c r="W7" t="n">
-        <v>1.541E12</v>
+        <v>1.5063229999999999</v>
       </c>
       <c r="X7" t="n">
-        <v>67.42423043569806</v>
+        <v>8.081422313109442</v>
       </c>
       <c r="Y7" t="n">
-        <v>1.161E12</v>
+        <v>18.270162</v>
       </c>
       <c r="Z7" t="n">
-        <v>48.24804871124627</v>
+        <v>105.40295252532087</v>
       </c>
       <c r="AA7" t="n">
-        <v>3.38E11</v>
+        <v>25.500705</v>
       </c>
       <c r="AB7" t="n">
-        <v>14.022177735268997</v>
+        <v>147.26799246913674</v>
       </c>
       <c r="AC7" t="n">
-        <v>3.638E12</v>
+        <v>11.730875</v>
       </c>
       <c r="AD7" t="n">
-        <v>146.47194732482444</v>
+        <v>67.9209411526881</v>
       </c>
       <c r="AE7" t="n">
-        <v>5.906E12</v>
+        <v>17.189411999999997</v>
       </c>
       <c r="AF7" t="n">
-        <v>143.93284876139376</v>
+        <v>74.41251456144437</v>
       </c>
       <c r="AG7" t="n">
-        <v>2.988E12</v>
+        <v>20.955993</v>
       </c>
       <c r="AH7" t="n">
-        <v>101.42902146610606</v>
+        <v>114.78784074629766</v>
       </c>
       <c r="AI7" t="n">
-        <v>3.862E12</v>
+        <v>30.500721999999996</v>
       </c>
       <c r="AJ7" t="n">
-        <v>105.40252714836492</v>
+        <v>95.2594686111363</v>
       </c>
       <c r="AK7" t="n">
-        <v>5.2284E13</v>
+        <v>359.68103099999996</v>
       </c>
       <c r="AL7" t="n">
-        <v>1835.633535505967</v>
+        <v>1838.1347314218806</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.454E12</v>
+        <v>31.6481</v>
       </c>
       <c r="B8" t="n">
-        <v>98.56426092704851</v>
+        <v>145.1218935355834</v>
       </c>
       <c r="C8" t="n">
-        <v>2.512E12</v>
+        <v>7.286651999999999</v>
       </c>
       <c r="D8" t="n">
-        <v>146.56558737304977</v>
+        <v>48.97109410667878</v>
       </c>
       <c r="E8" t="n">
-        <v>1.111E12</v>
+        <v>52.212289</v>
       </c>
       <c r="F8" t="n">
-        <v>49.42828140479463</v>
+        <v>304.52214602327695</v>
       </c>
       <c r="G8" t="n">
-        <v>3.579E12</v>
+        <v>12.160158999999998</v>
       </c>
       <c r="H8" t="n">
-        <v>143.9961520779833</v>
+        <v>35.62655013779846</v>
       </c>
       <c r="I8" t="n">
-        <v>2.876E12</v>
+        <v>18.963067</v>
       </c>
       <c r="J8" t="n">
-        <v>73.10663461743934</v>
+        <v>120.72093877599502</v>
       </c>
       <c r="K8" t="n">
-        <v>2.31E12</v>
+        <v>14.159572</v>
       </c>
       <c r="L8" t="n">
-        <v>35.522378857788624</v>
+        <v>103.66155893240807</v>
       </c>
       <c r="M8" t="n">
-        <v>4.305E12</v>
+        <v>24.78193</v>
       </c>
       <c r="N8" t="n">
-        <v>178.54857203621668</v>
+        <v>99.28548315553599</v>
       </c>
       <c r="O8" t="n">
-        <v>3.844E12</v>
+        <v>2.762311</v>
       </c>
       <c r="P8" t="n">
-        <v>96.58803754419569</v>
+        <v>13.428466352623673</v>
       </c>
       <c r="Q8" t="n">
-        <v>2.368E12</v>
+        <v>23.45749</v>
       </c>
       <c r="R8" t="n">
-        <v>103.11029675328712</v>
+        <v>144.8471941541626</v>
       </c>
       <c r="S8" t="n">
-        <v>2.585E12</v>
+        <v>4.037267</v>
       </c>
       <c r="T8" t="n">
-        <v>106.90803706588281</v>
+        <v>30.05331925941914</v>
       </c>
       <c r="U8" t="n">
-        <v>5.503E12</v>
+        <v>25.372959</v>
       </c>
       <c r="V8" t="n">
-        <v>146.1432241039273</v>
+        <v>178.6108032794839</v>
       </c>
       <c r="W8" t="n">
-        <v>3.38E11</v>
+        <v>1.129027</v>
       </c>
       <c r="X8" t="n">
-        <v>14.022177735268997</v>
+        <v>8.135976083101468</v>
       </c>
       <c r="Y8" t="n">
-        <v>1.78E12</v>
+        <v>15.20624</v>
       </c>
       <c r="Z8" t="n">
-        <v>68.17023112326615</v>
+        <v>104.08171668449927</v>
       </c>
       <c r="AA8" t="n">
-        <v>9.502E12</v>
+        <v>21.223482999999998</v>
       </c>
       <c r="AB8" t="n">
-        <v>304.1963452797172</v>
+        <v>148.67322172850345</v>
       </c>
       <c r="AC8" t="n">
-        <v>8.74E11</v>
+        <v>9.48655</v>
       </c>
       <c r="AD8" t="n">
-        <v>30.84932901784066</v>
+        <v>69.19470935197319</v>
       </c>
       <c r="AE8" t="n">
-        <v>4.196E12</v>
+        <v>15.821258</v>
       </c>
       <c r="AF8" t="n">
-        <v>114.787946261662</v>
+        <v>72.41604226610639</v>
       </c>
       <c r="AG8" t="n">
-        <v>3.803E12</v>
+        <v>19.137680999999997</v>
       </c>
       <c r="AH8" t="n">
-        <v>121.90747696169672</v>
+        <v>114.6652520191451</v>
       </c>
       <c r="AI8" t="n">
-        <v>2.08E11</v>
+        <v>23.002579</v>
       </c>
       <c r="AJ8" t="n">
-        <v>6.101985803477419</v>
+        <v>96.34544502282301</v>
       </c>
       <c r="AK8" t="n">
-        <v>5.3148E13</v>
+        <v>321.84861400000005</v>
       </c>
       <c r="AL8" t="n">
-        <v>1838.5169549445432</v>
+        <v>1838.3618108691178</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2.25E11</v>
+        <v>32.328117</v>
       </c>
       <c r="B9" t="n">
-        <v>14.426896677450259</v>
+        <v>145.25614353818875</v>
       </c>
       <c r="C9" t="n">
-        <v>1.814E12</v>
+        <v>8.859774999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>73.88080507054315</v>
+        <v>48.4052866354574</v>
       </c>
       <c r="E9" t="n">
-        <v>3.981E12</v>
+        <v>55.076405</v>
       </c>
       <c r="F9" t="n">
-        <v>122.9957142192859</v>
+        <v>304.5685409801994</v>
       </c>
       <c r="G9" t="n">
-        <v>2.708E12</v>
+        <v>14.046851999999998</v>
       </c>
       <c r="H9" t="n">
-        <v>106.19326311778377</v>
+        <v>35.217607437452045</v>
       </c>
       <c r="I9" t="n">
-        <v>1.176E12</v>
+        <v>21.345581</v>
       </c>
       <c r="J9" t="n">
-        <v>49.2842043518537</v>
+        <v>122.0978743592359</v>
       </c>
       <c r="K9" t="n">
-        <v>6.76E11</v>
+        <v>18.197062</v>
       </c>
       <c r="L9" t="n">
-        <v>29.138155252555293</v>
+        <v>103.31974129944854</v>
       </c>
       <c r="M9" t="n">
-        <v>3.844E12</v>
+        <v>16.578619999999997</v>
       </c>
       <c r="N9" t="n">
-        <v>96.58803754419569</v>
+        <v>99.55148700067275</v>
       </c>
       <c r="O9" t="n">
-        <v>2.254E12</v>
+        <v>2.373729</v>
       </c>
       <c r="P9" t="n">
-        <v>100.6827400343019</v>
+        <v>13.78117328790779</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.541E12</v>
+        <v>23.828367</v>
       </c>
       <c r="R9" t="n">
-        <v>67.42423043569806</v>
+        <v>144.5765167653584</v>
       </c>
       <c r="S9" t="n">
-        <v>2.65E12</v>
+        <v>4.732925</v>
       </c>
       <c r="T9" t="n">
-        <v>33.94666829474971</v>
+        <v>29.295326272308785</v>
       </c>
       <c r="U9" t="n">
-        <v>2.15E11</v>
+        <v>29.576106</v>
       </c>
       <c r="V9" t="n">
-        <v>8.015818833833237</v>
+        <v>179.29618106429484</v>
       </c>
       <c r="W9" t="n">
-        <v>5.906E12</v>
+        <v>1.142191</v>
       </c>
       <c r="X9" t="n">
-        <v>143.93284876139376</v>
+        <v>6.89310050762424</v>
       </c>
       <c r="Y9" t="n">
-        <v>4.087E12</v>
+        <v>17.745453</v>
       </c>
       <c r="Z9" t="n">
-        <v>143.67202261858745</v>
+        <v>107.18676679759551</v>
       </c>
       <c r="AA9" t="n">
-        <v>4.196E12</v>
+        <v>23.296805999999997</v>
       </c>
       <c r="AB9" t="n">
-        <v>114.787946261662</v>
+        <v>146.66249118413066</v>
       </c>
       <c r="AC9" t="n">
-        <v>2.799E12</v>
+        <v>10.367467999999999</v>
       </c>
       <c r="AD9" t="n">
-        <v>101.62843633765635</v>
+        <v>67.2445090767419</v>
       </c>
       <c r="AE9" t="n">
-        <v>3.988E12</v>
+        <v>16.193707999999997</v>
       </c>
       <c r="AF9" t="n">
-        <v>148.67223776130004</v>
+        <v>74.6863667001387</v>
       </c>
       <c r="AG9" t="n">
-        <v>1.005E13</v>
+        <v>20.018607</v>
       </c>
       <c r="AH9" t="n">
-        <v>304.5654343319479</v>
+        <v>114.2122081326745</v>
       </c>
       <c r="AI9" t="n">
-        <v>5.522E12</v>
+        <v>19.638324</v>
       </c>
       <c r="AJ9" t="n">
-        <v>177.41183656894555</v>
+        <v>96.0722346005416</v>
       </c>
       <c r="AK9" t="n">
-        <v>5.7632E13</v>
+        <v>335.34609599999993</v>
       </c>
       <c r="AL9" t="n">
-        <v>1837.247296473744</v>
+        <v>1838.3235556399718</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2.163E12</v>
+        <v>30.098482</v>
       </c>
       <c r="B10" t="n">
-        <v>144.14075436299777</v>
+        <v>144.85652664314452</v>
       </c>
       <c r="C10" t="n">
-        <v>2.663E12</v>
+        <v>7.117962</v>
       </c>
       <c r="D10" t="n">
-        <v>95.1878964172281</v>
+        <v>49.407288205707715</v>
       </c>
       <c r="E10" t="n">
-        <v>3.6E11</v>
+        <v>48.588486</v>
       </c>
       <c r="F10" t="n">
-        <v>12.769546349331335</v>
+        <v>304.46754157974055</v>
       </c>
       <c r="G10" t="n">
-        <v>3.417E12</v>
+        <v>12.327376</v>
       </c>
       <c r="H10" t="n">
-        <v>115.20492014937258</v>
+        <v>35.37840346966453</v>
       </c>
       <c r="I10" t="n">
-        <v>2.494E12</v>
+        <v>18.397969999999997</v>
       </c>
       <c r="J10" t="n">
-        <v>99.82806549513418</v>
+        <v>120.74406521413357</v>
       </c>
       <c r="K10" t="n">
-        <v>2.47E12</v>
+        <v>14.008914999999998</v>
       </c>
       <c r="L10" t="n">
-        <v>72.94929513009538</v>
+        <v>103.90360683293409</v>
       </c>
       <c r="M10" t="n">
-        <v>2.368E12</v>
+        <v>13.116268</v>
       </c>
       <c r="N10" t="n">
-        <v>103.11029675328712</v>
+        <v>99.93291347102513</v>
       </c>
       <c r="O10" t="n">
-        <v>1.541E12</v>
+        <v>1.5250219999999999</v>
       </c>
       <c r="P10" t="n">
-        <v>67.42423043569806</v>
+        <v>10.941281681734722</v>
       </c>
       <c r="Q10" t="n">
-        <v>4.209E12</v>
+        <v>19.262414999999997</v>
       </c>
       <c r="R10" t="n">
-        <v>122.3151680453899</v>
+        <v>145.7580969574036</v>
       </c>
       <c r="S10" t="n">
-        <v>3.638E12</v>
+        <v>3.6826969999999997</v>
       </c>
       <c r="T10" t="n">
-        <v>146.47194732482444</v>
+        <v>30.856240518838376</v>
       </c>
       <c r="U10" t="n">
-        <v>2.51E12</v>
+        <v>47.361137</v>
       </c>
       <c r="V10" t="n">
-        <v>35.24828070571334</v>
+        <v>182.001813303561</v>
       </c>
       <c r="W10" t="n">
-        <v>3.862E12</v>
+        <v>1.165414</v>
       </c>
       <c r="X10" t="n">
-        <v>105.40252714836492</v>
+        <v>7.1478137615240485</v>
       </c>
       <c r="Y10" t="n">
-        <v>9.458E12</v>
+        <v>13.596427</v>
       </c>
       <c r="Z10" t="n">
-        <v>303.7753036717446</v>
+        <v>107.23134818530866</v>
       </c>
       <c r="AA10" t="n">
-        <v>2.08E11</v>
+        <v>18.762622999999998</v>
       </c>
       <c r="AB10" t="n">
-        <v>6.101985803477419</v>
+        <v>147.94644017819792</v>
       </c>
       <c r="AC10" t="n">
-        <v>1.433E12</v>
+        <v>8.828332999999999</v>
       </c>
       <c r="AD10" t="n">
-        <v>48.405244981889155</v>
+        <v>67.5327693605243</v>
       </c>
       <c r="AE10" t="n">
-        <v>5.522E12</v>
+        <v>13.301728</v>
       </c>
       <c r="AF10" t="n">
-        <v>177.41183656894555</v>
+        <v>74.01019533098724</v>
       </c>
       <c r="AG10" t="n">
-        <v>5.37E12</v>
+        <v>16.606164999999997</v>
       </c>
       <c r="AH10" t="n">
-        <v>144.75602592194625</v>
+        <v>115.17198344112944</v>
       </c>
       <c r="AI10" t="n">
-        <v>6.09E11</v>
+        <v>16.1566</v>
       </c>
       <c r="AJ10" t="n">
-        <v>30.856491669416073</v>
+        <v>96.00620159225946</v>
       </c>
       <c r="AK10" t="n">
-        <v>5.4295E13</v>
+        <v>303.90402000000006</v>
       </c>
       <c r="AL10" t="n">
-        <v>1831.3598169348563</v>
+        <v>1843.294529727819</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4.36E11</v>
+        <v>22.335272999999997</v>
       </c>
       <c r="B11" t="n">
-        <v>30.402374312591405</v>
+        <v>144.0559171042507</v>
       </c>
       <c r="C11" t="n">
-        <v>4.541E12</v>
+        <v>4.839707</v>
       </c>
       <c r="D11" t="n">
-        <v>144.82315115315194</v>
+        <v>50.1539042226575</v>
       </c>
       <c r="E11" t="n">
-        <v>4.491E12</v>
+        <v>32.719642</v>
       </c>
       <c r="F11" t="n">
-        <v>178.7719518253857</v>
+        <v>304.27411787448335</v>
       </c>
       <c r="G11" t="n">
-        <v>1.176E12</v>
+        <v>11.10694</v>
       </c>
       <c r="H11" t="n">
-        <v>49.2842043518537</v>
+        <v>34.2381817216762</v>
       </c>
       <c r="I11" t="n">
-        <v>2.01E11</v>
+        <v>14.693862</v>
       </c>
       <c r="J11" t="n">
-        <v>7.8608007431755595</v>
+        <v>121.92382705667796</v>
       </c>
       <c r="K11" t="n">
-        <v>7.947E12</v>
+        <v>9.603344</v>
       </c>
       <c r="L11" t="n">
-        <v>305.0251841267425</v>
+        <v>103.25721586539419</v>
       </c>
       <c r="M11" t="n">
-        <v>2.585E12</v>
+        <v>9.427551</v>
       </c>
       <c r="N11" t="n">
-        <v>106.90803706588281</v>
+        <v>101.26835252606509</v>
       </c>
       <c r="O11" t="n">
-        <v>2.65E12</v>
+        <v>1.407166</v>
       </c>
       <c r="P11" t="n">
-        <v>33.94666829474971</v>
+        <v>14.993797343779306</v>
       </c>
       <c r="Q11" t="n">
-        <v>3.638E12</v>
+        <v>13.824842999999998</v>
       </c>
       <c r="R11" t="n">
-        <v>146.47194732482444</v>
+        <v>139.82333917025744</v>
       </c>
       <c r="S11" t="n">
-        <v>3.576E12</v>
+        <v>2.6460929999999996</v>
       </c>
       <c r="T11" t="n">
-        <v>120.98628599720064</v>
+        <v>30.095182276361243</v>
       </c>
       <c r="U11" t="n">
-        <v>2.612E12</v>
+        <v>16.479945999999998</v>
       </c>
       <c r="V11" t="n">
-        <v>67.92092063077212</v>
+        <v>179.4965965573981</v>
       </c>
       <c r="W11" t="n">
-        <v>2.799E12</v>
+        <v>0.78045</v>
       </c>
       <c r="X11" t="n">
-        <v>101.62843633765635</v>
+        <v>8.331930850672506</v>
       </c>
       <c r="Y11" t="n">
-        <v>2.686E12</v>
+        <v>9.763988999999999</v>
       </c>
       <c r="Z11" t="n">
-        <v>73.96540074344853</v>
+        <v>105.34457319608077</v>
       </c>
       <c r="AA11" t="n">
-        <v>3.054E12</v>
+        <v>14.011664</v>
       </c>
       <c r="AB11" t="n">
-        <v>99.55141903831475</v>
+        <v>148.51852853312926</v>
       </c>
       <c r="AC11" t="n">
-        <v>3.849E12</v>
+        <v>6.37102</v>
       </c>
       <c r="AD11" t="n">
-        <v>113.51814544924991</v>
+        <v>68.36997456838071</v>
       </c>
       <c r="AE11" t="n">
-        <v>2.64E11</v>
+        <v>9.352214</v>
       </c>
       <c r="AF11" t="n">
-        <v>12.764699232305361</v>
+        <v>72.67488052943577</v>
       </c>
       <c r="AG11" t="n">
-        <v>1.856E12</v>
+        <v>11.691601</v>
       </c>
       <c r="AH11" t="n">
-        <v>96.81952399545412</v>
+        <v>115.5820275242072</v>
       </c>
       <c r="AI11" t="n">
-        <v>2.171E12</v>
+        <v>12.232664</v>
       </c>
       <c r="AJ11" t="n">
-        <v>146.48795783081948</v>
+        <v>93.99381307879912</v>
       </c>
       <c r="AK11" t="n">
-        <v>5.0532E13</v>
+        <v>203.28796899999998</v>
       </c>
       <c r="AL11" t="n">
-        <v>1837.137108453579</v>
+        <v>1836.3961599997065</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:O19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>29.015902699999998</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4.949643979630051</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>145.46788393971198</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1.5728948302857697</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>6.746380499999999</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.539041480857501</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="n">
+        <v>49.123514364117014</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.557858375888854</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>47.081971800000005</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7.394899735210299</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" t="n">
+        <v>303.9999202371473</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1.4242748866430652</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>15.7327804</v>
+      </c>
+      <c r="C5" t="n">
+        <v>7.3672266177585195</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" t="n">
+        <v>34.61749096553595</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.6299248994712768</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="n">
+        <v>19.731995599999998</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3.20318439755813</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" t="n">
+        <v>121.84721037921426</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.8289402722004907</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="n">
+        <v>14.317458199999999</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2.4522057554688512</v>
+      </c>
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" t="n">
+        <v>103.78884974653224</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.5982677899941091</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="n">
+        <v>14.797235599999999</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3.93436297064768</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" t="n">
+        <v>99.70827885915281</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.856184822069391</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.9733647</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.44831425983478373</v>
+      </c>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" t="n">
+        <v>13.077229210510087</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1.67419724430878</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20.036779399999997</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.1081020080554693</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" t="n">
+        <v>144.12910823156136</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1.5613755182032303</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3.8580963999999995</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.5741992842979169</v>
+      </c>
+      <c r="J11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" t="n">
+        <v>30.253480696024997</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.6536409853072114</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="n">
+        <v>29.7428464</v>
+      </c>
+      <c r="C12" t="n">
+        <v>8.5629042822442</v>
+      </c>
+      <c r="J12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" t="n">
+        <v>178.83664595063053</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1.4574272021265928</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1.1808827000000002</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.18802098747908436</v>
+      </c>
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" t="n">
+        <v>7.822384146670993</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.8672632587640479</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="n">
+        <v>14.783157799999998</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2.2599324568024066</v>
+      </c>
+      <c r="J14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" t="n">
+        <v>105.95753333493039</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1.0399584041782284</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="n">
+        <v>20.136880899999998</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3.046038501297987</v>
+      </c>
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" t="n">
+        <v>147.36993030648392</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1.2407065880893802</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="n">
+        <v>9.3177246</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1.3920696287705008</v>
+      </c>
+      <c r="J16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" t="n">
+        <v>68.3958369358943</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1.1012781313071924</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="n">
+        <v>14.426066400000002</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2.199939105604525</v>
+      </c>
+      <c r="J17" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" t="n">
+        <v>73.50953456002719</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.7339243004955475</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="n">
+        <v>18.0014526</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2.526146132202458</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" t="n">
+        <v>115.0308340525336</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.524028959704376</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="n">
+        <v>21.7198475</v>
+      </c>
+      <c r="C19" t="n">
+        <v>6.29666330787747</v>
+      </c>
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" t="n">
+        <v>95.3578979230037</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.8518590884119736</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculo preliminar de bias e Gráficos de Dispersão
</commit_message>
<xml_diff>
--- a/ReconciliationReport.xlsx
+++ b/ReconciliationReport.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
   <si>
     <t>t1</t>
   </si>
@@ -129,6 +129,9 @@
     <t>dTOTAL</t>
   </si>
   <si>
+    <t>Tempos</t>
+  </si>
+  <si>
     <t>Médias</t>
   </si>
   <si>
@@ -142,6 +145,9 @@
   </si>
   <si>
     <t>Incerteza</t>
+  </si>
+  <si>
+    <t>Distâncias</t>
   </si>
 </sst>
 </file>
@@ -11922,35 +11928,41 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+      <c r="M1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" t="s">
+      <c r="N1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" t="s">
-        <v>41</v>
-      </c>
       <c r="O1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2">
@@ -11963,6 +11975,9 @@
       <c r="C2" t="n">
         <v>3.189630369855844</v>
       </c>
+      <c r="D2" t="n">
+        <v>5.811908301411682</v>
+      </c>
       <c r="J2" t="s">
         <v>1</v>
       </c>
@@ -11971,6 +11986,9 @@
       </c>
       <c r="L2" t="n">
         <v>0.7642848072141035</v>
+      </c>
+      <c r="M2" t="n">
+        <v>189.93238486058337</v>
       </c>
     </row>
     <row r="3">
@@ -11983,6 +12001,9 @@
       <c r="C3" t="n">
         <v>0.8070044851184138</v>
       </c>
+      <c r="D3" t="n">
+        <v>5.242603186250202</v>
+      </c>
       <c r="J3" t="s">
         <v>3</v>
       </c>
@@ -11991,6 +12012,9 @@
       </c>
       <c r="L3" t="n">
         <v>0.8047579749943305</v>
+      </c>
+      <c r="M3" t="n">
+        <v>61.32003693297221</v>
       </c>
     </row>
     <row r="4">
@@ -12003,6 +12027,9 @@
       <c r="C4" t="n">
         <v>3.8141291423717854</v>
       </c>
+      <c r="D4" t="n">
+        <v>7.444415751309205</v>
+      </c>
       <c r="J4" t="s">
         <v>5</v>
       </c>
@@ -12011,6 +12038,9 @@
       </c>
       <c r="L4" t="n">
         <v>0.6306219963742803</v>
+      </c>
+      <c r="M4" t="n">
+        <v>482.03278173822827</v>
       </c>
     </row>
     <row r="5">
@@ -12023,6 +12053,9 @@
       <c r="C5" t="n">
         <v>4.621457087065917</v>
       </c>
+      <c r="D5" t="n">
+        <v>1.9826198333948344</v>
+      </c>
       <c r="J5" t="s">
         <v>7</v>
       </c>
@@ -12031,6 +12064,9 @@
       </c>
       <c r="L5" t="n">
         <v>0.5829511310949792</v>
+      </c>
+      <c r="M5" t="n">
+        <v>59.9434371299528</v>
       </c>
     </row>
     <row r="6">
@@ -12043,6 +12079,9 @@
       <c r="C6" t="n">
         <v>1.8540360760604249</v>
       </c>
+      <c r="D6" t="n">
+        <v>6.261796070154588</v>
+      </c>
       <c r="J6" t="s">
         <v>9</v>
       </c>
@@ -12051,6 +12090,9 @@
       </c>
       <c r="L6" t="n">
         <v>0.9206227751036921</v>
+      </c>
+      <c r="M6" t="n">
+        <v>132.51902385524113</v>
       </c>
     </row>
     <row r="7">
@@ -12063,6 +12105,9 @@
       <c r="C7" t="n">
         <v>1.1314968750849086</v>
       </c>
+      <c r="D7" t="n">
+        <v>7.560919361229354</v>
+      </c>
       <c r="J7" t="s">
         <v>11</v>
       </c>
@@ -12071,6 +12116,9 @@
       </c>
       <c r="L7" t="n">
         <v>0.8223146163490254</v>
+      </c>
+      <c r="M7" t="n">
+        <v>125.85499102631753</v>
       </c>
     </row>
     <row r="8">
@@ -12083,6 +12131,9 @@
       <c r="C8" t="n">
         <v>3.6071305859636404</v>
       </c>
+      <c r="D8" t="n">
+        <v>2.562662157552723</v>
+      </c>
       <c r="J8" t="s">
         <v>13</v>
       </c>
@@ -12091,6 +12142,9 @@
       </c>
       <c r="L8" t="n">
         <v>0.757683779421013</v>
+      </c>
+      <c r="M8" t="n">
+        <v>131.9076158656049</v>
       </c>
     </row>
     <row r="9">
@@ -12103,6 +12157,9 @@
       <c r="C9" t="n">
         <v>0.9821548084495219</v>
       </c>
+      <c r="D9" t="n">
+        <v>1.2768962328655702</v>
+      </c>
       <c r="J9" t="s">
         <v>15</v>
       </c>
@@ -12111,6 +12168,9 @@
       </c>
       <c r="L9" t="n">
         <v>0.7883006303543195</v>
+      </c>
+      <c r="M9" t="n">
+        <v>17.3440837548009</v>
       </c>
     </row>
     <row r="10">
@@ -12123,6 +12183,9 @@
       <c r="C10" t="n">
         <v>1.594866243075226</v>
       </c>
+      <c r="D10" t="n">
+        <v>7.52429237379876</v>
+      </c>
       <c r="J10" t="s">
         <v>17</v>
       </c>
@@ -12131,6 +12194,9 @@
       </c>
       <c r="L10" t="n">
         <v>0.8285189964201444</v>
+      </c>
+      <c r="M10" t="n">
+        <v>173.60967122272027</v>
       </c>
     </row>
     <row r="11">
@@ -12143,6 +12209,9 @@
       <c r="C11" t="n">
         <v>0.3616125196900454</v>
       </c>
+      <c r="D11" t="n">
+        <v>6.532903222003773</v>
+      </c>
       <c r="J11" t="s">
         <v>19</v>
       </c>
@@ -12151,6 +12220,9 @@
       </c>
       <c r="L11" t="n">
         <v>0.8697307657755095</v>
+      </c>
+      <c r="M11" t="n">
+        <v>34.39581636650691</v>
       </c>
     </row>
     <row r="12">
@@ -12163,6 +12235,9 @@
       <c r="C12" t="n">
         <v>59.17153521762272</v>
       </c>
+      <c r="D12" t="n">
+        <v>0.3789389516857098</v>
+      </c>
       <c r="J12" t="s">
         <v>21</v>
       </c>
@@ -12171,6 +12246,9 @@
       </c>
       <c r="L12" t="n">
         <v>1.3186318918184137</v>
+      </c>
+      <c r="M12" t="n">
+        <v>135.42732905762406</v>
       </c>
     </row>
     <row r="13">
@@ -12183,6 +12261,9 @@
       <c r="C13" t="n">
         <v>2.423535157149635</v>
       </c>
+      <c r="D13" t="n">
+        <v>0.5069546531542815</v>
+      </c>
       <c r="J13" t="s">
         <v>23</v>
       </c>
@@ -12191,6 +12272,9 @@
       </c>
       <c r="L13" t="n">
         <v>0.9273997149831456</v>
+      </c>
+      <c r="M13" t="n">
+        <v>8.471998280856907</v>
       </c>
     </row>
     <row r="14">
@@ -12203,6 +12287,9 @@
       <c r="C14" t="n">
         <v>1.4212257534214987</v>
       </c>
+      <c r="D14" t="n">
+        <v>6.340497118987606</v>
+      </c>
       <c r="J14" t="s">
         <v>25</v>
       </c>
@@ -12211,6 +12298,9 @@
       </c>
       <c r="L14" t="n">
         <v>1.7253407692449685</v>
+      </c>
+      <c r="M14" t="n">
+        <v>61.83682895660404</v>
       </c>
     </row>
     <row r="15">
@@ -12223,6 +12313,9 @@
       <c r="C15" t="n">
         <v>3.500390322693855</v>
       </c>
+      <c r="D15" t="n">
+        <v>3.672296858342176</v>
+      </c>
       <c r="J15" t="s">
         <v>27</v>
       </c>
@@ -12231,6 +12324,9 @@
       </c>
       <c r="L15" t="n">
         <v>0.9278139372561025</v>
+      </c>
+      <c r="M15" t="n">
+        <v>158.39616828009542</v>
       </c>
     </row>
     <row r="16">
@@ -12243,6 +12339,9 @@
       <c r="C16" t="n">
         <v>0.7343170127585327</v>
       </c>
+      <c r="D16" t="n">
+        <v>7.737952840905323</v>
+      </c>
       <c r="J16" t="s">
         <v>29</v>
       </c>
@@ -12251,6 +12350,9 @@
       </c>
       <c r="L16" t="n">
         <v>0.8710700689712251</v>
+      </c>
+      <c r="M16" t="n">
+        <v>78.53331113293923</v>
       </c>
     </row>
     <row r="17">
@@ -12263,6 +12365,9 @@
       <c r="C17" t="n">
         <v>0.9738746695215263</v>
       </c>
+      <c r="D17" t="n">
+        <v>8.933512029093487</v>
+      </c>
       <c r="J17" t="s">
         <v>31</v>
       </c>
@@ -12271,6 +12376,9 @@
       </c>
       <c r="L17" t="n">
         <v>0.7006777265398245</v>
+      </c>
+      <c r="M17" t="n">
+        <v>104.82218314264418</v>
       </c>
     </row>
     <row r="18">
@@ -12283,6 +12391,9 @@
       <c r="C18" t="n">
         <v>1.1142653705132943</v>
       </c>
+      <c r="D18" t="n">
+        <v>9.877384195229897</v>
+      </c>
       <c r="J18" t="s">
         <v>33</v>
       </c>
@@ -12291,6 +12402,9 @@
       </c>
       <c r="L18" t="n">
         <v>0.6918040902975048</v>
+      </c>
+      <c r="M18" t="n">
+        <v>166.22249418525263</v>
       </c>
     </row>
     <row r="19">
@@ -12303,6 +12417,9 @@
       <c r="C19" t="n">
         <v>2.7513336187515063</v>
       </c>
+      <c r="D19" t="n">
+        <v>4.3959905253105465</v>
+      </c>
       <c r="J19" t="s">
         <v>35</v>
       </c>
@@ -12311,6 +12428,9 @@
       </c>
       <c r="L19" t="n">
         <v>0.7963402431448204</v>
+      </c>
+      <c r="M19" t="n">
+        <v>120.04217938861542</v>
       </c>
     </row>
     <row r="20">
@@ -12323,6 +12443,9 @@
       <c r="C20" t="n">
         <v>63.6747859847844</v>
       </c>
+      <c r="D20" t="n">
+        <v>2.958006096400666</v>
+      </c>
       <c r="J20" t="s">
         <v>37</v>
       </c>
@@ -12331,6 +12454,9 @@
       </c>
       <c r="L20" t="n">
         <v>1.721817338830316</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1067.9575065621536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reconciliação de Dados concluído e Bias corrigido
</commit_message>
<xml_diff>
--- a/ReconciliationReport.xlsx
+++ b/ReconciliationReport.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>t1</t>
   </si>
@@ -138,6 +138,9 @@
     <t>Desvio Padrão</t>
   </si>
   <si>
+    <t>Reconciliado</t>
+  </si>
+  <si>
     <t>Polarização (bias)</t>
   </si>
   <si>
@@ -11921,7 +11924,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11946,8 +11949,11 @@
       <c r="F1" t="s">
         <v>43</v>
       </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K1" t="s">
         <v>39</v>
@@ -11963,6 +11969,9 @@
       </c>
       <c r="O1" t="s">
         <v>43</v>
+      </c>
+      <c r="P1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2">
@@ -11976,7 +11985,10 @@
         <v>3.189630369855844</v>
       </c>
       <c r="D2" t="n">
-        <v>5.811908301411682</v>
+        <v>18.537839224999992</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0</v>
       </c>
       <c r="J2" t="s">
         <v>1</v>
@@ -11988,7 +12000,10 @@
         <v>0.7642848072141035</v>
       </c>
       <c r="M2" t="n">
-        <v>189.93238486058337</v>
+        <v>145.16243614688585</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-2.842170943040401E-14</v>
       </c>
     </row>
     <row r="3">
@@ -12002,7 +12017,10 @@
         <v>0.8070044851184138</v>
       </c>
       <c r="D3" t="n">
-        <v>5.242603186250202</v>
+        <v>4.230804285</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
       </c>
       <c r="J3" t="s">
         <v>3</v>
@@ -12014,7 +12032,10 @@
         <v>0.8047579749943305</v>
       </c>
       <c r="M3" t="n">
-        <v>61.32003693297221</v>
+        <v>49.34778874875626</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-1.4210854715202004E-14</v>
       </c>
     </row>
     <row r="4">
@@ -12028,7 +12049,10 @@
         <v>3.8141291423717854</v>
       </c>
       <c r="D4" t="n">
-        <v>7.444415751309205</v>
+        <v>28.393963064999987</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-3.552713678800501E-15</v>
       </c>
       <c r="J4" t="s">
         <v>5</v>
@@ -12040,7 +12064,10 @@
         <v>0.6306219963742803</v>
       </c>
       <c r="M4" t="n">
-        <v>482.03278173822827</v>
+        <v>303.98047513760923</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -12054,7 +12081,10 @@
         <v>4.621457087065917</v>
       </c>
       <c r="D5" t="n">
-        <v>1.9826198333948344</v>
+        <v>9.16259248</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-3.552713678800501E-15</v>
       </c>
       <c r="J5" t="s">
         <v>7</v>
@@ -12066,7 +12096,10 @@
         <v>0.5829511310949792</v>
       </c>
       <c r="M5" t="n">
-        <v>59.9434371299528</v>
+        <v>34.944094476626745</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-1.4210854715202004E-14</v>
       </c>
     </row>
     <row r="6">
@@ -12080,7 +12113,10 @@
         <v>1.8540360760604249</v>
       </c>
       <c r="D6" t="n">
-        <v>6.261796070154588</v>
+        <v>11.609595815000002</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0</v>
       </c>
       <c r="J6" t="s">
         <v>9</v>
@@ -12092,7 +12128,10 @@
         <v>0.9206227751036921</v>
       </c>
       <c r="M6" t="n">
-        <v>132.51902385524113</v>
+        <v>122.00003149564448</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2.842170943040401E-14</v>
       </c>
     </row>
     <row r="7">
@@ -12106,7 +12145,10 @@
         <v>1.1314968750849086</v>
       </c>
       <c r="D7" t="n">
-        <v>7.560919361229354</v>
+        <v>8.555156629999995</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-1.7763568394002505E-15</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
@@ -12118,7 +12160,10 @@
         <v>0.8223146163490254</v>
       </c>
       <c r="M7" t="n">
-        <v>125.85499102631753</v>
+        <v>103.4923986614163</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-2.842170943040401E-14</v>
       </c>
     </row>
     <row r="8">
@@ -12132,7 +12177,10 @@
         <v>3.6071305859636404</v>
       </c>
       <c r="D8" t="n">
-        <v>2.562662157552723</v>
+        <v>9.24385705</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0</v>
       </c>
       <c r="J8" t="s">
         <v>13</v>
@@ -12144,7 +12192,10 @@
         <v>0.757683779421013</v>
       </c>
       <c r="M8" t="n">
-        <v>131.9076158656049</v>
+        <v>99.94426092346669</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -12158,7 +12209,10 @@
         <v>0.9821548084495219</v>
       </c>
       <c r="D9" t="n">
-        <v>1.2768962328655702</v>
+        <v>1.2541097750000003</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.220446049250313E-16</v>
       </c>
       <c r="J9" t="s">
         <v>15</v>
@@ -12170,7 +12224,10 @@
         <v>0.7883006303543195</v>
       </c>
       <c r="M9" t="n">
-        <v>17.3440837548009</v>
+        <v>13.67235215682766</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
@@ -12184,7 +12241,10 @@
         <v>1.594866243075226</v>
       </c>
       <c r="D10" t="n">
-        <v>7.52429237379876</v>
+        <v>12.000239910000007</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.552713678800501E-15</v>
       </c>
       <c r="J10" t="s">
         <v>17</v>
@@ -12196,7 +12256,10 @@
         <v>0.8285189964201444</v>
       </c>
       <c r="M10" t="n">
-        <v>173.60967122272027</v>
+        <v>143.8389105702794</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -12210,7 +12273,10 @@
         <v>0.3616125196900454</v>
       </c>
       <c r="D11" t="n">
-        <v>6.532903222003773</v>
+        <v>2.3623795949999997</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-4.440892098500626E-16</v>
       </c>
       <c r="J11" t="s">
         <v>19</v>
@@ -12222,7 +12288,10 @@
         <v>0.8697307657755095</v>
       </c>
       <c r="M11" t="n">
-        <v>34.39581636650691</v>
+        <v>29.91509970791585</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="12">
@@ -12236,7 +12305,10 @@
         <v>59.17153521762272</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3789389516857098</v>
+        <v>22.422399525</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-1.0658141036401503E-14</v>
       </c>
       <c r="J12" t="s">
         <v>21</v>
@@ -12248,7 +12320,10 @@
         <v>1.3186318918184137</v>
       </c>
       <c r="M12" t="n">
-        <v>135.42732905762406</v>
+        <v>178.5787951191696</v>
+      </c>
+      <c r="N12" t="n">
+        <v>-2.842170943040401E-14</v>
       </c>
     </row>
     <row r="13">
@@ -12262,7 +12337,10 @@
         <v>2.423535157149635</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5069546531542815</v>
+        <v>1.2286224250000002</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0</v>
       </c>
       <c r="J13" t="s">
         <v>23</v>
@@ -12274,7 +12352,10 @@
         <v>0.9273997149831456</v>
       </c>
       <c r="M13" t="n">
-        <v>8.471998280856907</v>
+        <v>7.856928791004396</v>
+      </c>
+      <c r="N13" t="n">
+        <v>8.881784197001252E-16</v>
       </c>
     </row>
     <row r="14">
@@ -12288,7 +12369,10 @@
         <v>1.4212257534214987</v>
       </c>
       <c r="D14" t="n">
-        <v>6.340497118987606</v>
+        <v>9.011277795000003</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.7763568394002505E-15</v>
       </c>
       <c r="J14" t="s">
         <v>25</v>
@@ -12300,7 +12384,10 @@
         <v>1.7253407692449685</v>
       </c>
       <c r="M14" t="n">
-        <v>61.83682895660404</v>
+        <v>106.68960203965672</v>
+      </c>
+      <c r="N14" t="n">
+        <v>-2.842170943040401E-14</v>
       </c>
     </row>
     <row r="15">
@@ -12314,7 +12401,10 @@
         <v>3.500390322693855</v>
       </c>
       <c r="D15" t="n">
-        <v>3.672296858342176</v>
+        <v>12.854472385</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0</v>
       </c>
       <c r="J15" t="s">
         <v>27</v>
@@ -12326,7 +12416,10 @@
         <v>0.9278139372561025</v>
       </c>
       <c r="M15" t="n">
-        <v>158.39616828009542</v>
+        <v>146.96217253823554</v>
+      </c>
+      <c r="N15" t="n">
+        <v>2.842170943040401E-14</v>
       </c>
     </row>
     <row r="16">
@@ -12340,7 +12433,10 @@
         <v>0.7343170127585327</v>
       </c>
       <c r="D16" t="n">
-        <v>7.737952840905323</v>
+        <v>5.682110414999999</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.0</v>
       </c>
       <c r="J16" t="s">
         <v>29</v>
@@ -12352,7 +12448,10 @@
         <v>0.8710700689712251</v>
       </c>
       <c r="M16" t="n">
-        <v>78.53331113293923</v>
+        <v>68.40801674510804</v>
+      </c>
+      <c r="N16" t="n">
+        <v>-1.4210854715202004E-14</v>
       </c>
     </row>
     <row r="17">
@@ -12366,7 +12465,10 @@
         <v>0.9738746695215263</v>
       </c>
       <c r="D17" t="n">
-        <v>8.933512029093487</v>
+        <v>8.700121075</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0</v>
       </c>
       <c r="J17" t="s">
         <v>31</v>
@@ -12378,7 +12480,10 @@
         <v>0.7006777265398245</v>
       </c>
       <c r="M17" t="n">
-        <v>104.82218314264418</v>
+        <v>73.44656897532904</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
@@ -12392,7 +12497,10 @@
         <v>1.1142653705132943</v>
       </c>
       <c r="D18" t="n">
-        <v>9.877384195229897</v>
+        <v>11.006027159999997</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-1.7763568394002505E-15</v>
       </c>
       <c r="J18" t="s">
         <v>33</v>
@@ -12404,7 +12512,10 @@
         <v>0.6918040902975048</v>
       </c>
       <c r="M18" t="n">
-        <v>166.22249418525263</v>
+        <v>114.99340137681098</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1.4210854715202004E-14</v>
       </c>
     </row>
     <row r="19">
@@ -12418,7 +12529,10 @@
         <v>2.7513336187515063</v>
       </c>
       <c r="D19" t="n">
-        <v>4.3959905253105465</v>
+        <v>12.094836520000001</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0</v>
       </c>
       <c r="J19" t="s">
         <v>35</v>
@@ -12430,7 +12544,10 @@
         <v>0.7963402431448204</v>
       </c>
       <c r="M19" t="n">
-        <v>120.04217938861542</v>
+        <v>95.59441832196416</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="20">
@@ -12444,7 +12561,10 @@
         <v>63.6747859847844</v>
       </c>
       <c r="D20" t="n">
-        <v>2.958006096400666</v>
+        <v>188.35040512999998</v>
+      </c>
+      <c r="E20" t="n">
+        <v>5.684341886080802E-14</v>
       </c>
       <c r="J20" t="s">
         <v>37</v>
@@ -12456,7 +12576,10 @@
         <v>1.721817338830316</v>
       </c>
       <c r="M20" t="n">
-        <v>1067.9575065621536</v>
+        <v>1838.8277519327066</v>
+      </c>
+      <c r="N20" t="n">
+        <v>-4.547473508864641E-13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculo das velocidades e incertezas finalizado
</commit_message>
<xml_diff>
--- a/ReconciliationReport.xlsx
+++ b/ReconciliationReport.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="TimeDistanceReport" r:id="rId3" sheetId="1"/>
     <sheet name="Statistics" r:id="rId4" sheetId="2"/>
+    <sheet name="Speeds" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="70">
   <si>
     <t>t1</t>
   </si>
@@ -152,6 +153,78 @@
   <si>
     <t>Distâncias</t>
   </si>
+  <si>
+    <t>Parciais</t>
+  </si>
+  <si>
+    <t>Velocidade</t>
+  </si>
+  <si>
+    <t>Unidade de medida</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>Km/h</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>v3</t>
+  </si>
+  <si>
+    <t>v4</t>
+  </si>
+  <si>
+    <t>v5</t>
+  </si>
+  <si>
+    <t>v6</t>
+  </si>
+  <si>
+    <t>v7</t>
+  </si>
+  <si>
+    <t>v8</t>
+  </si>
+  <si>
+    <t>v9</t>
+  </si>
+  <si>
+    <t>v10</t>
+  </si>
+  <si>
+    <t>v11</t>
+  </si>
+  <si>
+    <t>v12</t>
+  </si>
+  <si>
+    <t>v13</t>
+  </si>
+  <si>
+    <t>v14</t>
+  </si>
+  <si>
+    <t>v15</t>
+  </si>
+  <si>
+    <t>v16</t>
+  </si>
+  <si>
+    <t>v17</t>
+  </si>
+  <si>
+    <t>v18</t>
+  </si>
+  <si>
+    <t>vTOTAL</t>
+  </si>
 </sst>
 </file>
 
@@ -11990,6 +12063,12 @@
       <c r="E2" t="n">
         <v>0.0</v>
       </c>
+      <c r="F2" t="n">
+        <v>0.8279394738975656</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.31896303698558437</v>
+      </c>
       <c r="J2" t="s">
         <v>1</v>
       </c>
@@ -12004,6 +12083,12 @@
       </c>
       <c r="N2" t="n">
         <v>-2.842170943040401E-14</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.9947349684429329</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.07642848072141036</v>
       </c>
     </row>
     <row r="3">
@@ -12022,6 +12107,12 @@
       <c r="E3" t="n">
         <v>0.0</v>
       </c>
+      <c r="F3" t="n">
+        <v>0.8092550657614705</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.08070044851184138</v>
+      </c>
       <c r="J3" t="s">
         <v>3</v>
       </c>
@@ -12036,6 +12127,12 @@
       </c>
       <c r="N3" t="n">
         <v>-1.4210854715202004E-14</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.9836921168019993</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.08047579749943305</v>
       </c>
     </row>
     <row r="4">
@@ -12054,6 +12151,12 @@
       <c r="E4" t="n">
         <v>-3.552713678800501E-15</v>
       </c>
+      <c r="F4" t="n">
+        <v>0.8656711240470233</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.38141291423717855</v>
+      </c>
       <c r="J4" t="s">
         <v>5</v>
       </c>
@@ -12068,6 +12171,12 @@
       </c>
       <c r="N4" t="n">
         <v>0.0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.9979254522972608</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.06306219963742803</v>
       </c>
     </row>
     <row r="5">
@@ -12086,6 +12195,12 @@
       <c r="E5" t="n">
         <v>-3.552713678800501E-15</v>
       </c>
+      <c r="F5" t="n">
+        <v>0.49561686857146847</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.46214570870659166</v>
+      </c>
       <c r="J5" t="s">
         <v>7</v>
       </c>
@@ -12100,6 +12215,12 @@
       </c>
       <c r="N5" t="n">
         <v>-1.4210854715202004E-14</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.9833176065991666</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.05829511310949792</v>
       </c>
     </row>
     <row r="6">
@@ -12118,6 +12239,12 @@
       <c r="E6" t="n">
         <v>0.0</v>
       </c>
+      <c r="F6" t="n">
+        <v>0.8403014105224107</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1854036076060425</v>
+      </c>
       <c r="J6" t="s">
         <v>9</v>
       </c>
@@ -12132,6 +12259,12 @@
       </c>
       <c r="N6" t="n">
         <v>2.842170943040401E-14</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.9924539136275833</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.0920622775103692</v>
       </c>
     </row>
     <row r="7">
@@ -12150,6 +12283,12 @@
       <c r="E7" t="n">
         <v>-1.7763568394002505E-15</v>
       </c>
+      <c r="F7" t="n">
+        <v>0.8677409515663176</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.11314968750849086</v>
+      </c>
       <c r="J7" t="s">
         <v>11</v>
       </c>
@@ -12164,6 +12303,12 @@
       </c>
       <c r="N7" t="n">
         <v>-2.842170943040401E-14</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.9920543476913769</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.08223146163490254</v>
       </c>
     </row>
     <row r="8">
@@ -12182,6 +12327,12 @@
       <c r="E8" t="n">
         <v>0.0</v>
       </c>
+      <c r="F8" t="n">
+        <v>0.6097807910212502</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.36071305859636404</v>
+      </c>
       <c r="J8" t="s">
         <v>13</v>
       </c>
@@ -12196,6 +12347,12 @@
       </c>
       <c r="N8" t="n">
         <v>0.0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.9924189365910543</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.0757683779421013</v>
       </c>
     </row>
     <row r="9">
@@ -12214,6 +12371,12 @@
       <c r="E9" t="n">
         <v>2.220446049250313E-16</v>
       </c>
+      <c r="F9" t="n">
+        <v>0.21685100616529218</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.09821548084495219</v>
+      </c>
       <c r="J9" t="s">
         <v>15</v>
       </c>
@@ -12228,6 +12391,12 @@
       </c>
       <c r="N9" t="n">
         <v>0.0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.9423434518572826</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.07883006303543195</v>
       </c>
     </row>
     <row r="10">
@@ -12246,6 +12415,12 @@
       <c r="E10" t="n">
         <v>3.552713678800501E-15</v>
       </c>
+      <c r="F10" t="n">
+        <v>0.8670971368042236</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.1594866243075226</v>
+      </c>
       <c r="J10" t="s">
         <v>17</v>
       </c>
@@ -12260,6 +12435,12 @@
       </c>
       <c r="N10" t="n">
         <v>0.0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.9942399522275627</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.08285189964201443</v>
       </c>
     </row>
     <row r="11">
@@ -12278,6 +12459,12 @@
       <c r="E11" t="n">
         <v>-4.440892098500626E-16</v>
       </c>
+      <c r="F11" t="n">
+        <v>0.8469286983110581</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.036161251969004535</v>
+      </c>
       <c r="J11" t="s">
         <v>19</v>
       </c>
@@ -12292,6 +12479,12 @@
       </c>
       <c r="N11" t="n">
         <v>0.0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.9709266967428704</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.08697307657755095</v>
       </c>
     </row>
     <row r="12">
@@ -12310,6 +12503,12 @@
       <c r="E12" t="n">
         <v>-1.0658141036401503E-14</v>
       </c>
+      <c r="F12" t="n">
+        <v>-1.6389475021015927</v>
+      </c>
+      <c r="G12" t="n">
+        <v>5.9171535217622715</v>
+      </c>
       <c r="J12" t="s">
         <v>21</v>
       </c>
@@ -12324,6 +12523,12 @@
       </c>
       <c r="N12" t="n">
         <v>-2.842170943040401E-14</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.9926159660169145</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.13186318918184137</v>
       </c>
     </row>
     <row r="13">
@@ -12342,6 +12547,12 @@
       <c r="E13" t="n">
         <v>0.0</v>
       </c>
+      <c r="F13" t="n">
+        <v>-0.9725630167865726</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.2423535157149635</v>
+      </c>
       <c r="J13" t="s">
         <v>23</v>
       </c>
@@ -12356,6 +12567,12 @@
       </c>
       <c r="N13" t="n">
         <v>8.881784197001252E-16</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.881964093139682</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.09273997149831456</v>
       </c>
     </row>
     <row r="14">
@@ -12374,6 +12591,12 @@
       <c r="E14" t="n">
         <v>1.7763568394002505E-15</v>
       </c>
+      <c r="F14" t="n">
+        <v>0.8422836599033624</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.14212257534214986</v>
+      </c>
       <c r="J14" t="s">
         <v>25</v>
       </c>
@@ -12388,6 +12611,12 @@
       </c>
       <c r="N14" t="n">
         <v>-2.842170943040401E-14</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.9838284074899477</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.17253407692449685</v>
       </c>
     </row>
     <row r="15">
@@ -12406,6 +12635,12 @@
       <c r="E15" t="n">
         <v>0.0</v>
       </c>
+      <c r="F15" t="n">
+        <v>0.7276908598147915</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.3500390322693855</v>
+      </c>
       <c r="J15" t="s">
         <v>27</v>
       </c>
@@ -12420,6 +12655,12 @@
       </c>
       <c r="N15" t="n">
         <v>2.842170943040401E-14</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.9936867159675752</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.09278139372561026</v>
       </c>
     </row>
     <row r="16">
@@ -12438,6 +12679,12 @@
       <c r="E16" t="n">
         <v>0.0</v>
       </c>
+      <c r="F16" t="n">
+        <v>0.8707668526081374</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.07343170127585327</v>
+      </c>
       <c r="J16" t="s">
         <v>29</v>
       </c>
@@ -12452,6 +12699,12 @@
       </c>
       <c r="N16" t="n">
         <v>-1.4210854715202004E-14</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.9872665498808878</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.0871070068971225</v>
       </c>
     </row>
     <row r="17">
@@ -12470,6 +12723,12 @@
       <c r="E17" t="n">
         <v>0.0</v>
       </c>
+      <c r="F17" t="n">
+        <v>0.8880619406182774</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.09738746695215264</v>
+      </c>
       <c r="J17" t="s">
         <v>31</v>
       </c>
@@ -12484,6 +12743,12 @@
       </c>
       <c r="N17" t="n">
         <v>0.0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.9904600346031796</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.07006777265398245</v>
       </c>
     </row>
     <row r="18">
@@ -12502,6 +12767,12 @@
       <c r="E18" t="n">
         <v>-1.7763568394002505E-15</v>
       </c>
+      <c r="F18" t="n">
+        <v>0.8987586206798626</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.11142653705132943</v>
+      </c>
       <c r="J18" t="s">
         <v>33</v>
       </c>
@@ -12516,6 +12787,12 @@
       </c>
       <c r="N18" t="n">
         <v>1.4210854715202004E-14</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.9939839670623308</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.06918040902975048</v>
       </c>
     </row>
     <row r="19">
@@ -12534,6 +12811,12 @@
       <c r="E19" t="n">
         <v>0.0</v>
       </c>
+      <c r="F19" t="n">
+        <v>0.7725199828702185</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.27513336187515064</v>
+      </c>
       <c r="J19" t="s">
         <v>35</v>
       </c>
@@ -12548,6 +12831,12 @@
       </c>
       <c r="N19" t="n">
         <v>0.0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.9916695947616656</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.07963402431448205</v>
       </c>
     </row>
     <row r="20">
@@ -12566,6 +12855,12 @@
       <c r="E20" t="n">
         <v>5.684341886080802E-14</v>
       </c>
+      <c r="F20" t="n">
+        <v>0.6619344357617075</v>
+      </c>
+      <c r="G20" t="n">
+        <v>6.36747859847844</v>
+      </c>
       <c r="J20" t="s">
         <v>37</v>
       </c>
@@ -12580,6 +12875,545 @@
       </c>
       <c r="N20" t="n">
         <v>-4.547473508864641E-13</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.9990636331559491</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.1721817338830316</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="n">
+        <v>7.8306017430079375</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.13479680995366922</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" t="n">
+        <v>28.190166274828577</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.4852685158332092</v>
+      </c>
+      <c r="J2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="n">
+        <v>11.66392615317025</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.2232951265176375</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="n">
+        <v>41.9901341514129</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.803862455463495</v>
+      </c>
+      <c r="J3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="n">
+        <v>10.705813571769868</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.14382713942282638</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" t="n">
+        <v>38.54092885837152</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.517777701922175</v>
+      </c>
+      <c r="J4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3.8137780931436494</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.19246572091152098</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" t="n">
+        <v>13.729601135317138</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.6928765952814755</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="n">
+        <v>10.508551153694444</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.16800732590505751</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" t="n">
+        <v>37.8307841533</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.6048263732582071</v>
+      </c>
+      <c r="J6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="n">
+        <v>12.097078187733468</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.16028326982970245</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" t="n">
+        <v>43.54948147584049</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.5770197713869288</v>
+      </c>
+      <c r="J7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="n">
+        <v>10.811965220023245</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.4219832648037539</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" t="n">
+        <v>38.92307479208368</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.5191397532935143</v>
+      </c>
+      <c r="J8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="n">
+        <v>10.902037787583353</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.8561026908960923</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="n">
+        <v>39.24733603530007</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3.081969687225932</v>
+      </c>
+      <c r="J9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="n">
+        <v>11.986336244029252</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.15945138512317414</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" t="n">
+        <v>43.150810478505306</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.5740249864434269</v>
+      </c>
+      <c r="J10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="n">
+        <v>12.663121443832084</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.1973013492440464</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" t="n">
+        <v>45.5872371977955</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.710284857278567</v>
+      </c>
+      <c r="J11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="n">
+        <v>7.964303504629913</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2.1017461115599643</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" t="n">
+        <v>28.67149261666769</v>
+      </c>
+      <c r="I12" t="n">
+        <v>7.566286001615872</v>
+      </c>
+      <c r="J12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="n">
+        <v>6.39490915282976</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.2636925157621757</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" t="n">
+        <v>23.021672950187135</v>
+      </c>
+      <c r="I13" t="n">
+        <v>4.549293056743832</v>
+      </c>
+      <c r="J13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="n">
+        <v>11.839564206849166</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.1877083070725674</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" t="n">
+        <v>42.622431144657</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.6757499054612426</v>
+      </c>
+      <c r="J14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="n">
+        <v>11.432765821623844</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.3114083218386037</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" t="n">
+        <v>41.15795695784584</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1.1210699586189732</v>
+      </c>
+      <c r="J15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="n">
+        <v>12.039191734908949</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.15633968087451622</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" t="n">
+        <v>43.34109024567221</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.5628228511482584</v>
+      </c>
+      <c r="J16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="n">
+        <v>8.442016880245433</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.09484086572427858</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" t="n">
+        <v>30.39126076888356</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.3414271166074029</v>
+      </c>
+      <c r="J17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="n">
+        <v>10.448220752601797</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.10596581953184728</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" t="n">
+        <v>37.61359470936647</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.38147695031465023</v>
+      </c>
+      <c r="J18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="n">
+        <v>7.903737943368593</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.179914760636219</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" t="n">
+        <v>28.453456596126934</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.6476931382903884</v>
+      </c>
+      <c r="J19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="n">
+        <v>9.762802212522677</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.3300479898554693</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" t="n">
+        <v>35.14608796508164</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1.1881727634796895</v>
+      </c>
+      <c r="J20" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção Reconciliação de Dados
</commit_message>
<xml_diff>
--- a/ReconciliationReport.xlsx
+++ b/ReconciliationReport.xlsx
@@ -8983,10 +8983,10 @@
         <v>1.799355391222782</v>
       </c>
       <c r="D2" t="n">
-        <v>22.890123337500015</v>
+        <v>23.068616000000006</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0</v>
+        <v>0.17849266249999118</v>
       </c>
       <c r="F2" t="n">
         <v>0.9213916253445884</v>
@@ -9004,10 +9004,10 @@
         <v>0.4883568803382298</v>
       </c>
       <c r="M2" t="n">
-        <v>249.85104440418772</v>
+        <v>249.49278027131</v>
       </c>
       <c r="N2" t="n">
-        <v>-8.526512829121202E-14</v>
+        <v>-0.35826413287779246</v>
       </c>
       <c r="O2" t="n">
         <v>0.9980454078889172</v>
@@ -9027,10 +9027,10 @@
         <v>5.059942424652598</v>
       </c>
       <c r="D3" t="n">
-        <v>11.956933939999983</v>
+        <v>19.262699750000003</v>
       </c>
       <c r="E3" t="n">
-        <v>-8.881784197001252E-15</v>
+        <v>7.305765810000011</v>
       </c>
       <c r="F3" t="n">
         <v>0.576819404536026</v>
@@ -9048,10 +9048,10 @@
         <v>1.095668773156472</v>
       </c>
       <c r="M3" t="n">
-        <v>83.48635497060889</v>
+        <v>82.86328482501447</v>
       </c>
       <c r="N3" t="n">
-        <v>1.5631940186722204E-13</v>
+        <v>-0.6230701455942551</v>
       </c>
       <c r="O3" t="n">
         <v>0.9868760736584775</v>
@@ -9071,10 +9071,10 @@
         <v>1.2164429766103229</v>
       </c>
       <c r="D4" t="n">
-        <v>9.748775099999992</v>
+        <v>9.9607555</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0</v>
+        <v>0.21198040000000695</v>
       </c>
       <c r="F4" t="n">
         <v>0.8752209416944777</v>
@@ -9092,10 +9092,10 @@
         <v>1.3564775972946441</v>
       </c>
       <c r="M4" t="n">
-        <v>110.49230963008658</v>
+        <v>111.49631916740344</v>
       </c>
       <c r="N4" t="n">
-        <v>-7.105427357601002E-14</v>
+        <v>1.00400953731679</v>
       </c>
       <c r="O4" t="n">
         <v>0.9877233302314347</v>
@@ -9115,10 +9115,10 @@
         <v>9.093948867120314</v>
       </c>
       <c r="D5" t="n">
-        <v>12.524510424999994</v>
+        <v>19.964299749999977</v>
       </c>
       <c r="E5" t="n">
-        <v>-7.105427357601002E-15</v>
+        <v>7.4397893249999765</v>
       </c>
       <c r="F5" t="n">
         <v>0.27390783683105013</v>
@@ -9136,10 +9136,10 @@
         <v>1.547455125531464</v>
       </c>
       <c r="M5" t="n">
-        <v>73.47255216003701</v>
+        <v>72.429970090252</v>
       </c>
       <c r="N5" t="n">
-        <v>1.4210854715202004E-14</v>
+        <v>-1.0425820697849986</v>
       </c>
       <c r="O5" t="n">
         <v>0.9789383234958163</v>
@@ -9159,10 +9159,10 @@
         <v>13.869844530897643</v>
       </c>
       <c r="D6" t="n">
-        <v>45.45760064499999</v>
+        <v>36.52823000000003</v>
       </c>
       <c r="E6" t="n">
-        <v>7.105427357601002E-15</v>
+        <v>-8.929370644999956</v>
       </c>
       <c r="F6" t="n">
         <v>0.6948839284498569</v>
@@ -9180,10 +9180,10 @@
         <v>5.570616981158772</v>
       </c>
       <c r="M6" t="n">
-        <v>29.58932303764021</v>
+        <v>31.213017707021226</v>
       </c>
       <c r="N6" t="n">
-        <v>7.105427357601002E-15</v>
+        <v>1.623694669381024</v>
       </c>
       <c r="O6" t="n">
         <v>0.811735571845545</v>
@@ -9203,10 +9203,10 @@
         <v>0.3330831548381837</v>
       </c>
       <c r="D7" t="n">
-        <v>4.940559745000002</v>
+        <v>5.190070000000002</v>
       </c>
       <c r="E7" t="n">
-        <v>8.881784197001252E-16</v>
+        <v>0.24951025500000146</v>
       </c>
       <c r="F7" t="n">
         <v>0.9325818992118708</v>
@@ -9224,10 +9224,10 @@
         <v>1.3765975888974176</v>
       </c>
       <c r="M7" t="n">
-        <v>43.62586217512214</v>
+        <v>41.726392798285815</v>
       </c>
       <c r="N7" t="n">
-        <v>7.105427357601002E-15</v>
+        <v>-1.899469376836315</v>
       </c>
       <c r="O7" t="n">
         <v>0.9684453780335274</v>
@@ -9247,10 +9247,10 @@
         <v>1.4206161862099087</v>
       </c>
       <c r="D8" t="n">
-        <v>13.6325224275</v>
+        <v>13.219860749999997</v>
       </c>
       <c r="E8" t="n">
-        <v>1.7763568394002505E-15</v>
+        <v>-0.41266167750000093</v>
       </c>
       <c r="F8" t="n">
         <v>0.8957921255024535</v>
@@ -9268,10 +9268,10 @@
         <v>0.922325000887472</v>
       </c>
       <c r="M8" t="n">
-        <v>159.39164484627173</v>
+        <v>160.08442072665272</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0</v>
+        <v>0.6927758803809922</v>
       </c>
       <c r="O8" t="n">
         <v>0.9942134670749083</v>
@@ -9291,10 +9291,10 @@
         <v>0.8202229129198917</v>
       </c>
       <c r="D9" t="n">
-        <v>5.877986807500001</v>
+        <v>5.878192749999999</v>
       </c>
       <c r="E9" t="n">
-        <v>1.7763568394002505E-15</v>
+        <v>2.0594250000005587E-4</v>
       </c>
       <c r="F9" t="n">
         <v>0.8604585311635387</v>
@@ -9312,10 +9312,10 @@
         <v>0.9997952083060258</v>
       </c>
       <c r="M9" t="n">
-        <v>88.19200534460208</v>
+        <v>87.0194978827494</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0</v>
+        <v>-1.1725074618526747</v>
       </c>
       <c r="O9" t="n">
         <v>0.988663425846828</v>
@@ -9335,10 +9335,10 @@
         <v>4.438386934050192</v>
       </c>
       <c r="D10" t="n">
-        <v>41.77348661999999</v>
+        <v>48.48797575</v>
       </c>
       <c r="E10" t="n">
-        <v>7.105427357601002E-15</v>
+        <v>6.714489130000011</v>
       </c>
       <c r="F10" t="n">
         <v>0.8937511016395453</v>
@@ -9356,10 +9356,10 @@
         <v>1.0019416525493787</v>
       </c>
       <c r="M10" t="n">
-        <v>74.72324464510048</v>
+        <v>75.69028234346479</v>
       </c>
       <c r="N10" t="n">
-        <v>1.4210854715202004E-14</v>
+        <v>0.9670376983643223</v>
       </c>
       <c r="O10" t="n">
         <v>0.9865912989015918</v>
@@ -9379,10 +9379,10 @@
         <v>2.5759863737446898</v>
       </c>
       <c r="D11" t="n">
-        <v>16.967428684999998</v>
+        <v>19.225666000000004</v>
       </c>
       <c r="E11" t="n">
-        <v>-3.552713678800501E-15</v>
+        <v>2.2582373150000024</v>
       </c>
       <c r="F11" t="n">
         <v>0.8481805097538448</v>
@@ -9400,10 +9400,10 @@
         <v>0.6876061283844943</v>
       </c>
       <c r="M11" t="n">
-        <v>163.77207342906271</v>
+        <v>163.40211694872414</v>
       </c>
       <c r="N11" t="n">
-        <v>2.842170943040401E-14</v>
+        <v>-0.3699564803385442</v>
       </c>
       <c r="O11" t="n">
         <v>0.9958014445687389</v>
@@ -9423,10 +9423,10 @@
         <v>2.1308196229406713</v>
       </c>
       <c r="D12" t="n">
-        <v>4.565655342499997</v>
+        <v>4.1929412500000005</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0</v>
+        <v>-0.3727140924999963</v>
       </c>
       <c r="F12" t="n">
         <v>0.5332938071111808</v>
@@ -9444,10 +9444,10 @@
         <v>0.47496863635749725</v>
       </c>
       <c r="M12" t="n">
-        <v>26.231260753272437</v>
+        <v>26.03843802729898</v>
       </c>
       <c r="N12" t="n">
-        <v>-3.552713678800501E-15</v>
+        <v>-0.1928227259734605</v>
       </c>
       <c r="O12" t="n">
         <v>0.9818930305780958</v>
@@ -9467,10 +9467,10 @@
         <v>2.0703441533791143</v>
       </c>
       <c r="D13" t="n">
-        <v>12.18378028</v>
+        <v>12.41103225</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0</v>
+        <v>0.2272519699999993</v>
       </c>
       <c r="F13" t="n">
         <v>0.8300737451103218</v>
@@ -9488,10 +9488,10 @@
         <v>0.8497999538099986</v>
       </c>
       <c r="M13" t="n">
-        <v>154.23826944792486</v>
+        <v>153.6460497630287</v>
       </c>
       <c r="N13" t="n">
-        <v>2.842170943040401E-14</v>
+        <v>-0.5922196848961221</v>
       </c>
       <c r="O13" t="n">
         <v>0.994490343046173</v>
@@ -9511,10 +9511,10 @@
         <v>2.351838495747105</v>
       </c>
       <c r="D14" t="n">
-        <v>19.865063832499988</v>
+        <v>26.602334749999997</v>
       </c>
       <c r="E14" t="n">
-        <v>-3.552713678800501E-15</v>
+        <v>6.737270917500005</v>
       </c>
       <c r="F14" t="n">
         <v>0.8816093159540012</v>
@@ -9532,10 +9532,10 @@
         <v>0.793725850828756</v>
       </c>
       <c r="M14" t="n">
-        <v>161.46877060574644</v>
+        <v>161.95816477345215</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0</v>
+        <v>0.4893941677057114</v>
       </c>
       <c r="O14" t="n">
         <v>0.9950843383036168</v>
@@ -9555,10 +9555,10 @@
         <v>17.516660901849498</v>
       </c>
       <c r="D15" t="n">
-        <v>222.38442718749994</v>
+        <v>243.99267450000002</v>
       </c>
       <c r="E15" t="n">
-        <v>-1.1368683772161603E-13</v>
+        <v>21.60824731249997</v>
       </c>
       <c r="F15" t="n">
         <v>0.9212325200852279</v>
@@ -9576,10 +9576,10 @@
         <v>5.893024041317602</v>
       </c>
       <c r="M15" t="n">
-        <v>1418.5347154496633</v>
+        <v>1417.060735324658</v>
       </c>
       <c r="N15" t="n">
-        <v>2.2737367544323206E-13</v>
+        <v>-1.4739801250050277</v>
       </c>
       <c r="O15" t="n">
         <v>0.9958456962828368</v>
@@ -9632,10 +9632,10 @@
         <v>39</v>
       </c>
       <c r="B2" t="n">
-        <v>10.915233645546431</v>
+        <v>10.815247012274597</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08582939794485185</v>
+        <v>0.08438564180090444</v>
       </c>
       <c r="D2" t="s">
         <v>40</v>
@@ -9644,10 +9644,10 @@
         <v>39</v>
       </c>
       <c r="H2" t="n">
-        <v>39.29484112396715</v>
+        <v>38.93488924418855</v>
       </c>
       <c r="I2" t="n">
-        <v>0.30898583260146667</v>
+        <v>0.303788310483256</v>
       </c>
       <c r="J2" t="s">
         <v>41</v>
@@ -9658,10 +9658,10 @@
         <v>42</v>
       </c>
       <c r="B3" t="n">
-        <v>6.982254429901869</v>
+        <v>4.301748244039077</v>
       </c>
       <c r="C3" t="n">
-        <v>0.29561751588722246</v>
+        <v>0.11314175948563998</v>
       </c>
       <c r="D3" t="s">
         <v>40</v>
@@ -9670,10 +9670,10 @@
         <v>42</v>
       </c>
       <c r="H3" t="n">
-        <v>25.13611594764673</v>
+        <v>15.486293678540678</v>
       </c>
       <c r="I3" t="n">
-        <v>1.0642230571940008</v>
+        <v>0.4073103341483039</v>
       </c>
       <c r="J3" t="s">
         <v>41</v>
@@ -9684,10 +9684,10 @@
         <v>43</v>
       </c>
       <c r="B4" t="n">
-        <v>11.33396847262244</v>
+        <v>11.193560485186435</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1421070396073055</v>
+        <v>0.1373764100178965</v>
       </c>
       <c r="D4" t="s">
         <v>40</v>
@@ -9696,10 +9696,10 @@
         <v>43</v>
       </c>
       <c r="H4" t="n">
-        <v>40.80228650144078</v>
+        <v>40.29681774667117</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5115853425862998</v>
+        <v>0.4945550760644274</v>
       </c>
       <c r="J4" t="s">
         <v>41</v>
@@ -9710,10 +9710,10 @@
         <v>44</v>
       </c>
       <c r="B5" t="n">
-        <v>5.86630132970144</v>
+        <v>3.6279744843167907</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4261267006275125</v>
+        <v>0.16543973558617975</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -9722,10 +9722,10 @@
         <v>44</v>
       </c>
       <c r="H5" t="n">
-        <v>21.118684786925186</v>
+        <v>13.060708143540447</v>
       </c>
       <c r="I5" t="n">
-        <v>1.534056122259045</v>
+        <v>0.5955830481102471</v>
       </c>
       <c r="J5" t="s">
         <v>41</v>
@@ -9736,10 +9736,10 @@
         <v>45</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6509213556764092</v>
+        <v>0.8544902861984061</v>
       </c>
       <c r="C6" t="n">
-        <v>0.023337079508789795</v>
+        <v>0.03585048006609994</v>
       </c>
       <c r="D6" t="s">
         <v>40</v>
@@ -9748,10 +9748,10 @@
         <v>45</v>
       </c>
       <c r="H6" t="n">
-        <v>2.343316880435073</v>
+        <v>3.076165030314262</v>
       </c>
       <c r="I6" t="n">
-        <v>0.08401348623164326</v>
+        <v>0.1290617282379598</v>
       </c>
       <c r="J6" t="s">
         <v>41</v>
@@ -9762,10 +9762,10 @@
         <v>46</v>
       </c>
       <c r="B7" t="n">
-        <v>8.830145656931455</v>
+        <v>8.039658963807</v>
       </c>
       <c r="C7" t="n">
-        <v>0.06572911840982247</v>
+        <v>0.05801435753794925</v>
       </c>
       <c r="D7" t="s">
         <v>40</v>
@@ -9774,10 +9774,10 @@
         <v>46</v>
       </c>
       <c r="H7" t="n">
-        <v>31.78852436495324</v>
+        <v>28.9427722697052</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2366248262753609</v>
+        <v>0.2088516871366173</v>
       </c>
       <c r="J7" t="s">
         <v>41</v>
@@ -9788,10 +9788,10 @@
         <v>47</v>
       </c>
       <c r="B8" t="n">
-        <v>11.692014129735913</v>
+        <v>12.109387818374165</v>
       </c>
       <c r="C8" t="n">
-        <v>0.12202769280399667</v>
+        <v>0.1303152890754782</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
@@ -9800,10 +9800,10 @@
         <v>47</v>
       </c>
       <c r="H8" t="n">
-        <v>42.09125086704929</v>
+        <v>43.59379614614699</v>
       </c>
       <c r="I8" t="n">
-        <v>0.439299694094388</v>
+        <v>0.46913504067172157</v>
       </c>
       <c r="J8" t="s">
         <v>41</v>
@@ -9814,10 +9814,10 @@
         <v>48</v>
       </c>
       <c r="B9" t="n">
-        <v>15.003777353170262</v>
+        <v>14.803784357488007</v>
       </c>
       <c r="C9" t="n">
-        <v>0.21005470181532698</v>
+        <v>0.2072659958984005</v>
       </c>
       <c r="D9" t="s">
         <v>40</v>
@@ -9826,10 +9826,10 @@
         <v>48</v>
       </c>
       <c r="H9" t="n">
-        <v>54.01359847141295</v>
+        <v>53.29362368695683</v>
       </c>
       <c r="I9" t="n">
-        <v>0.7561969265351771</v>
+        <v>0.7461575852342418</v>
       </c>
       <c r="J9" t="s">
         <v>41</v>
@@ -9840,10 +9840,10 @@
         <v>49</v>
       </c>
       <c r="B10" t="n">
-        <v>1.7887720343966944</v>
+        <v>1.5610113883433212</v>
       </c>
       <c r="C10" t="n">
-        <v>0.019156255004242236</v>
+        <v>0.014437487048745134</v>
       </c>
       <c r="D10" t="s">
         <v>40</v>
@@ -9852,10 +9852,10 @@
         <v>49</v>
       </c>
       <c r="H10" t="n">
-        <v>6.4395793238281</v>
+        <v>5.6196409980359565</v>
       </c>
       <c r="I10" t="n">
-        <v>0.06896251801527205</v>
+        <v>0.05197495337548248</v>
       </c>
       <c r="J10" t="s">
         <v>41</v>
@@ -9866,10 +9866,10 @@
         <v>50</v>
       </c>
       <c r="B11" t="n">
-        <v>9.652144498113902</v>
+        <v>8.499165487880841</v>
       </c>
       <c r="C11" t="n">
-        <v>0.14659439090275825</v>
+        <v>0.1139337876947622</v>
       </c>
       <c r="D11" t="s">
         <v>40</v>
@@ -9878,10 +9878,10 @@
         <v>50</v>
       </c>
       <c r="H11" t="n">
-        <v>34.74772019321005</v>
+        <v>30.59699575637103</v>
       </c>
       <c r="I11" t="n">
-        <v>0.5277398072499297</v>
+        <v>0.41016163570114395</v>
       </c>
       <c r="J11" t="s">
         <v>41</v>
@@ -9892,10 +9892,10 @@
         <v>51</v>
       </c>
       <c r="B12" t="n">
-        <v>5.745344049318689</v>
+        <v>6.2100650771815555</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2683404948988057</v>
+        <v>0.31579383682221224</v>
       </c>
       <c r="D12" t="s">
         <v>40</v>
@@ -9904,10 +9904,10 @@
         <v>51</v>
       </c>
       <c r="H12" t="n">
-        <v>20.683238577547282</v>
+        <v>22.356234277853602</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9660257816357005</v>
+        <v>1.136857812559964</v>
       </c>
       <c r="J12" t="s">
         <v>41</v>
@@ -9918,10 +9918,10 @@
         <v>52</v>
       </c>
       <c r="B13" t="n">
-        <v>12.65931147011171</v>
+        <v>12.37979619004122</v>
       </c>
       <c r="C13" t="n">
-        <v>0.21522798460981027</v>
+        <v>0.20662683177290783</v>
       </c>
       <c r="D13" t="s">
         <v>40</v>
@@ -9930,10 +9930,10 @@
         <v>52</v>
       </c>
       <c r="H13" t="n">
-        <v>45.573521292402155</v>
+        <v>44.567266284148396</v>
       </c>
       <c r="I13" t="n">
-        <v>0.774820744595317</v>
+        <v>0.7438565943824682</v>
       </c>
       <c r="J13" t="s">
         <v>41</v>
@@ -9944,10 +9944,10 @@
         <v>53</v>
       </c>
       <c r="B14" t="n">
-        <v>8.128278467526366</v>
+        <v>6.088118441312831</v>
       </c>
       <c r="C14" t="n">
-        <v>0.09631415880727211</v>
+        <v>0.05390599909432408</v>
       </c>
       <c r="D14" t="s">
         <v>40</v>
@@ -9956,10 +9956,10 @@
         <v>53</v>
       </c>
       <c r="H14" t="n">
-        <v>29.261802483094918</v>
+        <v>21.917226388726192</v>
       </c>
       <c r="I14" t="n">
-        <v>0.3467309717061796</v>
+        <v>0.1940615967395667</v>
       </c>
       <c r="J14" t="s">
         <v>41</v>
@@ -9970,10 +9970,10 @@
         <v>54</v>
       </c>
       <c r="B15" t="n">
-        <v>6.378750227207448</v>
+        <v>5.807800329368733</v>
       </c>
       <c r="C15" t="n">
-        <v>0.050313639872884085</v>
+        <v>0.041765108948216785</v>
       </c>
       <c r="D15" t="s">
         <v>40</v>
@@ -9982,10 +9982,10 @@
         <v>54</v>
       </c>
       <c r="H15" t="n">
-        <v>22.963500817946812</v>
+        <v>20.908081185727436</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1811291035423827</v>
+        <v>0.15035439221358043</v>
       </c>
       <c r="J15" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Gráfico de linha e início do escalonamento
</commit_message>
<xml_diff>
--- a/ReconciliationReport.xlsx
+++ b/ReconciliationReport.xlsx
@@ -8983,10 +8983,10 @@
         <v>1.799355391222782</v>
       </c>
       <c r="D2" t="n">
-        <v>23.068616000000006</v>
+        <v>24.02015624999999</v>
       </c>
       <c r="E2" t="n">
-        <v>0.17849266249999118</v>
+        <v>1.1300329124999742</v>
       </c>
       <c r="F2" t="n">
         <v>0.9213916253445884</v>
@@ -9004,10 +9004,10 @@
         <v>0.4883568803382298</v>
       </c>
       <c r="M2" t="n">
-        <v>249.49278027131</v>
+        <v>250.15039088411143</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.35826413287779246</v>
+        <v>0.29934647992362784</v>
       </c>
       <c r="O2" t="n">
         <v>0.9980454078889172</v>
@@ -9027,10 +9027,10 @@
         <v>5.059942424652598</v>
       </c>
       <c r="D3" t="n">
-        <v>19.262699750000003</v>
+        <v>8.031721500000014</v>
       </c>
       <c r="E3" t="n">
-        <v>7.305765810000011</v>
+        <v>-3.925212439999978</v>
       </c>
       <c r="F3" t="n">
         <v>0.576819404536026</v>
@@ -9048,10 +9048,10 @@
         <v>1.095668773156472</v>
       </c>
       <c r="M3" t="n">
-        <v>82.86328482501447</v>
+        <v>83.57307479169685</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.6230701455942551</v>
+        <v>0.08671982108812415</v>
       </c>
       <c r="O3" t="n">
         <v>0.9868760736584775</v>
@@ -9071,10 +9071,10 @@
         <v>1.2164429766103229</v>
       </c>
       <c r="D4" t="n">
-        <v>9.9607555</v>
+        <v>10.241316000000003</v>
       </c>
       <c r="E4" t="n">
-        <v>0.21198040000000695</v>
+        <v>0.4925409000000105</v>
       </c>
       <c r="F4" t="n">
         <v>0.8752209416944777</v>
@@ -9092,10 +9092,10 @@
         <v>1.3564775972946441</v>
       </c>
       <c r="M4" t="n">
-        <v>111.49631916740344</v>
+        <v>109.13106377294746</v>
       </c>
       <c r="N4" t="n">
-        <v>1.00400953731679</v>
+        <v>-1.3612458571391954</v>
       </c>
       <c r="O4" t="n">
         <v>0.9877233302314347</v>
@@ -9115,10 +9115,10 @@
         <v>9.093948867120314</v>
       </c>
       <c r="D5" t="n">
-        <v>19.964299749999977</v>
+        <v>7.503612499999992</v>
       </c>
       <c r="E5" t="n">
-        <v>7.4397893249999765</v>
+        <v>-5.020897925000009</v>
       </c>
       <c r="F5" t="n">
         <v>0.27390783683105013</v>
@@ -9136,10 +9136,10 @@
         <v>1.547455125531464</v>
       </c>
       <c r="M5" t="n">
-        <v>72.429970090252</v>
+        <v>73.62914792002994</v>
       </c>
       <c r="N5" t="n">
-        <v>-1.0425820697849986</v>
+        <v>0.15659575999293907</v>
       </c>
       <c r="O5" t="n">
         <v>0.9789383234958163</v>
@@ -9159,10 +9159,10 @@
         <v>13.869844530897643</v>
       </c>
       <c r="D6" t="n">
-        <v>36.52823000000003</v>
+        <v>41.679207</v>
       </c>
       <c r="E6" t="n">
-        <v>-8.929370644999956</v>
+        <v>-3.778393644999987</v>
       </c>
       <c r="F6" t="n">
         <v>0.6948839284498569</v>
@@ -9180,10 +9180,10 @@
         <v>5.570616981158772</v>
       </c>
       <c r="M6" t="n">
-        <v>31.213017707021226</v>
+        <v>33.935730261306304</v>
       </c>
       <c r="N6" t="n">
-        <v>1.623694669381024</v>
+        <v>4.346407223666102</v>
       </c>
       <c r="O6" t="n">
         <v>0.811735571845545</v>
@@ -9203,10 +9203,10 @@
         <v>0.3330831548381837</v>
       </c>
       <c r="D7" t="n">
-        <v>5.190070000000002</v>
+        <v>5.256855249999999</v>
       </c>
       <c r="E7" t="n">
-        <v>0.24951025500000146</v>
+        <v>0.3162955049999985</v>
       </c>
       <c r="F7" t="n">
         <v>0.9325818992118708</v>
@@ -9224,10 +9224,10 @@
         <v>1.3765975888974176</v>
       </c>
       <c r="M7" t="n">
-        <v>41.726392798285815</v>
+        <v>45.30763442388707</v>
       </c>
       <c r="N7" t="n">
-        <v>-1.899469376836315</v>
+        <v>1.6817722487649434</v>
       </c>
       <c r="O7" t="n">
         <v>0.9684453780335274</v>
@@ -9247,10 +9247,10 @@
         <v>1.4206161862099087</v>
       </c>
       <c r="D8" t="n">
-        <v>13.219860749999997</v>
+        <v>15.226627750000002</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.41266167750000093</v>
+        <v>1.5941053225000044</v>
       </c>
       <c r="F8" t="n">
         <v>0.8957921255024535</v>
@@ -9268,10 +9268,10 @@
         <v>0.922325000887472</v>
       </c>
       <c r="M8" t="n">
-        <v>160.08442072665272</v>
+        <v>158.97508123642908</v>
       </c>
       <c r="N8" t="n">
-        <v>0.6927758803809922</v>
+        <v>-0.4165636098426546</v>
       </c>
       <c r="O8" t="n">
         <v>0.9942134670749083</v>
@@ -9291,10 +9291,10 @@
         <v>0.8202229129198917</v>
       </c>
       <c r="D9" t="n">
-        <v>5.878192749999999</v>
+        <v>6.249899499999999</v>
       </c>
       <c r="E9" t="n">
-        <v>2.0594250000005587E-4</v>
+        <v>0.3719126924999996</v>
       </c>
       <c r="F9" t="n">
         <v>0.8604585311635387</v>
@@ -9312,10 +9312,10 @@
         <v>0.9997952083060258</v>
       </c>
       <c r="M9" t="n">
-        <v>87.0194978827494</v>
+        <v>87.64042093754689</v>
       </c>
       <c r="N9" t="n">
-        <v>-1.1725074618526747</v>
+        <v>-0.5515844070551879</v>
       </c>
       <c r="O9" t="n">
         <v>0.988663425846828</v>
@@ -9335,10 +9335,10 @@
         <v>4.438386934050192</v>
       </c>
       <c r="D10" t="n">
-        <v>48.48797575</v>
+        <v>45.03974074999999</v>
       </c>
       <c r="E10" t="n">
-        <v>6.714489130000011</v>
+        <v>3.266254130000007</v>
       </c>
       <c r="F10" t="n">
         <v>0.8937511016395453</v>
@@ -9356,10 +9356,10 @@
         <v>1.0019416525493787</v>
       </c>
       <c r="M10" t="n">
-        <v>75.69028234346479</v>
+        <v>75.00178929657703</v>
       </c>
       <c r="N10" t="n">
-        <v>0.9670376983643223</v>
+        <v>0.27854465147656526</v>
       </c>
       <c r="O10" t="n">
         <v>0.9865912989015918</v>
@@ -9379,10 +9379,10 @@
         <v>2.5759863737446898</v>
       </c>
       <c r="D11" t="n">
-        <v>19.225666000000004</v>
+        <v>18.959232249999996</v>
       </c>
       <c r="E11" t="n">
-        <v>2.2582373150000024</v>
+        <v>1.9918035649999943</v>
       </c>
       <c r="F11" t="n">
         <v>0.8481805097538448</v>
@@ -9400,10 +9400,10 @@
         <v>0.6876061283844943</v>
       </c>
       <c r="M11" t="n">
-        <v>163.40211694872414</v>
+        <v>163.78093162494042</v>
       </c>
       <c r="N11" t="n">
-        <v>-0.3699564803385442</v>
+        <v>0.008858195877735398</v>
       </c>
       <c r="O11" t="n">
         <v>0.9958014445687389</v>
@@ -9423,10 +9423,10 @@
         <v>2.1308196229406713</v>
       </c>
       <c r="D12" t="n">
-        <v>4.1929412500000005</v>
+        <v>4.0894685</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.3727140924999963</v>
+        <v>-0.4761868424999971</v>
       </c>
       <c r="F12" t="n">
         <v>0.5332938071111808</v>
@@ -9444,10 +9444,10 @@
         <v>0.47496863635749725</v>
       </c>
       <c r="M12" t="n">
-        <v>26.03843802729898</v>
+        <v>26.648822360846676</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.1928227259734605</v>
+        <v>0.41756160757423544</v>
       </c>
       <c r="O12" t="n">
         <v>0.9818930305780958</v>
@@ -9467,10 +9467,10 @@
         <v>2.0703441533791143</v>
       </c>
       <c r="D13" t="n">
-        <v>12.41103225</v>
+        <v>13.502141249999998</v>
       </c>
       <c r="E13" t="n">
-        <v>0.2272519699999993</v>
+        <v>1.318360969999997</v>
       </c>
       <c r="F13" t="n">
         <v>0.8300737451103218</v>
@@ -9488,10 +9488,10 @@
         <v>0.8497999538099986</v>
       </c>
       <c r="M13" t="n">
-        <v>153.6460497630287</v>
+        <v>153.46252723917135</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.5922196848961221</v>
+        <v>-0.7757422087534849</v>
       </c>
       <c r="O13" t="n">
         <v>0.994490343046173</v>
@@ -9511,10 +9511,10 @@
         <v>2.351838495747105</v>
       </c>
       <c r="D14" t="n">
-        <v>26.602334749999997</v>
+        <v>22.4719305</v>
       </c>
       <c r="E14" t="n">
-        <v>6.737270917500005</v>
+        <v>2.6068666675000074</v>
       </c>
       <c r="F14" t="n">
         <v>0.8816093159540012</v>
@@ -9532,10 +9532,10 @@
         <v>0.793725850828756</v>
       </c>
       <c r="M14" t="n">
-        <v>161.95816477345215</v>
+        <v>161.93272048892686</v>
       </c>
       <c r="N14" t="n">
-        <v>0.4893941677057114</v>
+        <v>0.46394988318041896</v>
       </c>
       <c r="O14" t="n">
         <v>0.9950843383036168</v>
@@ -9555,10 +9555,10 @@
         <v>17.516660901849498</v>
       </c>
       <c r="D15" t="n">
-        <v>243.99267450000002</v>
+        <v>222.27190900000002</v>
       </c>
       <c r="E15" t="n">
-        <v>21.60824731249997</v>
+        <v>-0.1125181875000294</v>
       </c>
       <c r="F15" t="n">
         <v>0.9212325200852279</v>
@@ -9576,10 +9576,10 @@
         <v>5.893024041317602</v>
       </c>
       <c r="M15" t="n">
-        <v>1417.060735324658</v>
+        <v>1423.169335238417</v>
       </c>
       <c r="N15" t="n">
-        <v>-1.4739801250050277</v>
+        <v>4.63461978875398</v>
       </c>
       <c r="O15" t="n">
         <v>0.9958456962828368</v>
@@ -9632,10 +9632,10 @@
         <v>39</v>
       </c>
       <c r="B2" t="n">
-        <v>10.815247012274597</v>
+        <v>10.414186663923617</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08438564180090444</v>
+        <v>0.07803939839340147</v>
       </c>
       <c r="D2" t="s">
         <v>40</v>
@@ -9644,10 +9644,10 @@
         <v>39</v>
       </c>
       <c r="H2" t="n">
-        <v>38.93488924418855</v>
+        <v>37.49107199012502</v>
       </c>
       <c r="I2" t="n">
-        <v>0.303788310483256</v>
+        <v>0.2809418342162453</v>
       </c>
       <c r="J2" t="s">
         <v>41</v>
@@ -9658,10 +9658,10 @@
         <v>42</v>
       </c>
       <c r="B3" t="n">
-        <v>4.301748244039077</v>
+        <v>10.405375085739303</v>
       </c>
       <c r="C3" t="n">
-        <v>0.11314175948563998</v>
+        <v>0.6556751020613024</v>
       </c>
       <c r="D3" t="s">
         <v>40</v>
@@ -9670,10 +9670,10 @@
         <v>42</v>
       </c>
       <c r="H3" t="n">
-        <v>15.486293678540678</v>
+        <v>37.45935030866149</v>
       </c>
       <c r="I3" t="n">
-        <v>0.4073103341483039</v>
+        <v>2.3604303674206886</v>
       </c>
       <c r="J3" t="s">
         <v>41</v>
@@ -9684,10 +9684,10 @@
         <v>43</v>
       </c>
       <c r="B4" t="n">
-        <v>11.193560485186435</v>
+        <v>10.655960989090408</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1373764100178965</v>
+        <v>0.1272605155492091</v>
       </c>
       <c r="D4" t="s">
         <v>40</v>
@@ -9696,10 +9696,10 @@
         <v>43</v>
       </c>
       <c r="H4" t="n">
-        <v>40.29681774667117</v>
+        <v>38.36145956072547</v>
       </c>
       <c r="I4" t="n">
-        <v>0.4945550760644274</v>
+        <v>0.45813785597715284</v>
       </c>
       <c r="J4" t="s">
         <v>41</v>
@@ -9710,10 +9710,10 @@
         <v>44</v>
       </c>
       <c r="B5" t="n">
-        <v>3.6279744843167907</v>
+        <v>9.812493371696634</v>
       </c>
       <c r="C5" t="n">
-        <v>0.16543973558617975</v>
+        <v>1.1893968345811738</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -9722,10 +9722,10 @@
         <v>44</v>
       </c>
       <c r="H5" t="n">
-        <v>13.060708143540447</v>
+        <v>35.324976138107886</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5955830481102471</v>
+        <v>4.281828604492226</v>
       </c>
       <c r="J5" t="s">
         <v>41</v>
@@ -9736,10 +9736,10 @@
         <v>45</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8544902861984061</v>
+        <v>0.8142124743713647</v>
       </c>
       <c r="C6" t="n">
-        <v>0.03585048006609994</v>
+        <v>0.030212199628910322</v>
       </c>
       <c r="D6" t="s">
         <v>40</v>
@@ -9748,10 +9748,10 @@
         <v>45</v>
       </c>
       <c r="H6" t="n">
-        <v>3.076165030314262</v>
+        <v>2.931164907736913</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1290617282379598</v>
+        <v>0.10876391866407716</v>
       </c>
       <c r="J6" t="s">
         <v>41</v>
@@ -9762,10 +9762,10 @@
         <v>46</v>
       </c>
       <c r="B7" t="n">
-        <v>8.039658963807</v>
+        <v>8.61877154100583</v>
       </c>
       <c r="C7" t="n">
-        <v>0.05801435753794925</v>
+        <v>0.0605639651641692</v>
       </c>
       <c r="D7" t="s">
         <v>40</v>
@@ -9774,10 +9774,10 @@
         <v>46</v>
       </c>
       <c r="H7" t="n">
-        <v>28.9427722697052</v>
+        <v>31.027577547620986</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2088516871366173</v>
+        <v>0.21803027459100913</v>
       </c>
       <c r="J7" t="s">
         <v>41</v>
@@ -9788,10 +9788,10 @@
         <v>47</v>
       </c>
       <c r="B8" t="n">
-        <v>12.109387818374165</v>
+        <v>10.440596818059669</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1303152890754782</v>
+        <v>0.09759698963529764</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
@@ -9800,10 +9800,10 @@
         <v>47</v>
       </c>
       <c r="H8" t="n">
-        <v>43.59379614614699</v>
+        <v>37.58614854501481</v>
       </c>
       <c r="I8" t="n">
-        <v>0.46913504067172157</v>
+        <v>0.3513491626870715</v>
       </c>
       <c r="J8" t="s">
         <v>41</v>
@@ -9814,10 +9814,10 @@
         <v>48</v>
       </c>
       <c r="B9" t="n">
-        <v>14.803784357488007</v>
+        <v>14.022692834908291</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2072659958984005</v>
+        <v>0.18472466781855088</v>
       </c>
       <c r="D9" t="s">
         <v>40</v>
@@ -9826,10 +9826,10 @@
         <v>48</v>
       </c>
       <c r="H9" t="n">
-        <v>53.29362368695683</v>
+        <v>50.48169420566985</v>
       </c>
       <c r="I9" t="n">
-        <v>0.7461575852342418</v>
+        <v>0.6650088041467832</v>
       </c>
       <c r="J9" t="s">
         <v>41</v>
@@ -9840,10 +9840,10 @@
         <v>49</v>
       </c>
       <c r="B10" t="n">
-        <v>1.5610113883433212</v>
+        <v>1.6652358128099802</v>
       </c>
       <c r="C10" t="n">
-        <v>0.014437487048745134</v>
+        <v>0.01655996400472885</v>
       </c>
       <c r="D10" t="s">
         <v>40</v>
@@ -9852,10 +9852,10 @@
         <v>49</v>
       </c>
       <c r="H10" t="n">
-        <v>5.6196409980359565</v>
+        <v>5.994848926115929</v>
       </c>
       <c r="I10" t="n">
-        <v>0.05197495337548248</v>
+        <v>0.05961587041702386</v>
       </c>
       <c r="J10" t="s">
         <v>41</v>
@@ -9866,10 +9866,10 @@
         <v>50</v>
       </c>
       <c r="B11" t="n">
-        <v>8.499165487880841</v>
+        <v>8.638584593790208</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1139337876947622</v>
+        <v>0.11742826275302161</v>
       </c>
       <c r="D11" t="s">
         <v>40</v>
@@ -9878,10 +9878,10 @@
         <v>50</v>
       </c>
       <c r="H11" t="n">
-        <v>30.59699575637103</v>
+        <v>31.09890453764475</v>
       </c>
       <c r="I11" t="n">
-        <v>0.41016163570114395</v>
+        <v>0.4227417459108778</v>
       </c>
       <c r="J11" t="s">
         <v>41</v>
@@ -9892,10 +9892,10 @@
         <v>51</v>
       </c>
       <c r="B12" t="n">
-        <v>6.2100650771815555</v>
+        <v>6.51645130922189</v>
       </c>
       <c r="C12" t="n">
-        <v>0.31579383682221224</v>
+        <v>0.33973860967753566</v>
       </c>
       <c r="D12" t="s">
         <v>40</v>
@@ -9904,10 +9904,10 @@
         <v>51</v>
       </c>
       <c r="H12" t="n">
-        <v>22.356234277853602</v>
+        <v>23.459224713198804</v>
       </c>
       <c r="I12" t="n">
-        <v>1.136857812559964</v>
+        <v>1.2230589948391284</v>
       </c>
       <c r="J12" t="s">
         <v>41</v>
@@ -9918,10 +9918,10 @@
         <v>52</v>
       </c>
       <c r="B13" t="n">
-        <v>12.37979619004122</v>
+        <v>11.365791869431924</v>
       </c>
       <c r="C13" t="n">
-        <v>0.20662683177290783</v>
+        <v>0.17439041783941456</v>
       </c>
       <c r="D13" t="s">
         <v>40</v>
@@ -9930,10 +9930,10 @@
         <v>52</v>
       </c>
       <c r="H13" t="n">
-        <v>44.567266284148396</v>
+        <v>40.91685072995492</v>
       </c>
       <c r="I13" t="n">
-        <v>0.7438565943824682</v>
+        <v>0.6278055042218924</v>
       </c>
       <c r="J13" t="s">
         <v>41</v>
@@ -9944,10 +9944,10 @@
         <v>53</v>
       </c>
       <c r="B14" t="n">
-        <v>6.088118441312831</v>
+        <v>7.205999524114177</v>
       </c>
       <c r="C14" t="n">
-        <v>0.05390599909432408</v>
+        <v>0.07549829286370431</v>
       </c>
       <c r="D14" t="s">
         <v>40</v>
@@ -9956,10 +9956,10 @@
         <v>53</v>
       </c>
       <c r="H14" t="n">
-        <v>21.917226388726192</v>
+        <v>25.94159828681104</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1940615967395667</v>
+        <v>0.2717938543093355</v>
       </c>
       <c r="J14" t="s">
         <v>41</v>
@@ -9970,10 +9970,10 @@
         <v>54</v>
       </c>
       <c r="B15" t="n">
-        <v>5.807800329368733</v>
+        <v>6.402830396523102</v>
       </c>
       <c r="C15" t="n">
-        <v>0.041765108948216785</v>
+        <v>0.050528616619386534</v>
       </c>
       <c r="D15" t="s">
         <v>40</v>
@@ -9982,10 +9982,10 @@
         <v>54</v>
       </c>
       <c r="H15" t="n">
-        <v>20.908081185727436</v>
+        <v>23.05018942748317</v>
       </c>
       <c r="I15" t="n">
-        <v>0.15035439221358043</v>
+        <v>0.1819030198297915</v>
       </c>
       <c r="J15" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Testes unitários adicionados e comentários
</commit_message>
<xml_diff>
--- a/ReconciliationReport.xlsx
+++ b/ReconciliationReport.xlsx
@@ -8983,10 +8983,10 @@
         <v>1.799355391222782</v>
       </c>
       <c r="D2" t="n">
-        <v>24.02015624999999</v>
+        <v>22.575200000000002</v>
       </c>
       <c r="E2" t="n">
-        <v>1.1300329124999742</v>
+        <v>-0.3149233375000122</v>
       </c>
       <c r="F2" t="n">
         <v>0.9213916253445884</v>
@@ -9004,10 +9004,10 @@
         <v>0.4883568803382298</v>
       </c>
       <c r="M2" t="n">
-        <v>250.15039088411143</v>
+        <v>250.11335994715682</v>
       </c>
       <c r="N2" t="n">
-        <v>0.29934647992362784</v>
+        <v>0.26231554296902004</v>
       </c>
       <c r="O2" t="n">
         <v>0.9980454078889172</v>
@@ -9027,10 +9027,10 @@
         <v>5.059942424652598</v>
       </c>
       <c r="D3" t="n">
-        <v>8.031721500000014</v>
+        <v>20.640013500000016</v>
       </c>
       <c r="E3" t="n">
-        <v>-3.925212439999978</v>
+        <v>8.683079560000024</v>
       </c>
       <c r="F3" t="n">
         <v>0.576819404536026</v>
@@ -9048,10 +9048,10 @@
         <v>1.095668773156472</v>
       </c>
       <c r="M3" t="n">
-        <v>83.57307479169685</v>
+        <v>84.45377269046827</v>
       </c>
       <c r="N3" t="n">
-        <v>0.08671982108812415</v>
+        <v>0.9674177198595402</v>
       </c>
       <c r="O3" t="n">
         <v>0.9868760736584775</v>
@@ -9071,10 +9071,10 @@
         <v>1.2164429766103229</v>
       </c>
       <c r="D4" t="n">
-        <v>10.241316000000003</v>
+        <v>9.746518250000001</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4925409000000105</v>
+        <v>-0.002256849999991317</v>
       </c>
       <c r="F4" t="n">
         <v>0.8752209416944777</v>
@@ -9092,10 +9092,10 @@
         <v>1.3564775972946441</v>
       </c>
       <c r="M4" t="n">
-        <v>109.13106377294746</v>
+        <v>113.13687585280597</v>
       </c>
       <c r="N4" t="n">
-        <v>-1.3612458571391954</v>
+        <v>2.6445662227193196</v>
       </c>
       <c r="O4" t="n">
         <v>0.9877233302314347</v>
@@ -9115,10 +9115,10 @@
         <v>9.093948867120314</v>
       </c>
       <c r="D5" t="n">
-        <v>7.503612499999992</v>
+        <v>6.911729999999988</v>
       </c>
       <c r="E5" t="n">
-        <v>-5.020897925000009</v>
+        <v>-5.612780425000013</v>
       </c>
       <c r="F5" t="n">
         <v>0.27390783683105013</v>
@@ -9136,10 +9136,10 @@
         <v>1.547455125531464</v>
       </c>
       <c r="M5" t="n">
-        <v>73.62914792002994</v>
+        <v>73.40306221563604</v>
       </c>
       <c r="N5" t="n">
-        <v>0.15659575999293907</v>
+        <v>-0.06948994440095646</v>
       </c>
       <c r="O5" t="n">
         <v>0.9789383234958163</v>
@@ -9159,10 +9159,10 @@
         <v>13.869844530897643</v>
       </c>
       <c r="D6" t="n">
-        <v>41.679207</v>
+        <v>48.13514399999998</v>
       </c>
       <c r="E6" t="n">
-        <v>-3.778393644999987</v>
+        <v>2.6775433549999974</v>
       </c>
       <c r="F6" t="n">
         <v>0.6948839284498569</v>
@@ -9180,10 +9180,10 @@
         <v>5.570616981158772</v>
       </c>
       <c r="M6" t="n">
-        <v>33.935730261306304</v>
+        <v>34.27482010611674</v>
       </c>
       <c r="N6" t="n">
-        <v>4.346407223666102</v>
+        <v>4.68549706847654</v>
       </c>
       <c r="O6" t="n">
         <v>0.811735571845545</v>
@@ -9203,10 +9203,10 @@
         <v>0.3330831548381837</v>
       </c>
       <c r="D7" t="n">
-        <v>5.256855249999999</v>
+        <v>5.065843999999999</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3162955049999985</v>
+        <v>0.12528425499999862</v>
       </c>
       <c r="F7" t="n">
         <v>0.9325818992118708</v>
@@ -9224,10 +9224,10 @@
         <v>1.3765975888974176</v>
       </c>
       <c r="M7" t="n">
-        <v>45.30763442388707</v>
+        <v>44.198782873567325</v>
       </c>
       <c r="N7" t="n">
-        <v>1.6817722487649434</v>
+        <v>0.5729206984451949</v>
       </c>
       <c r="O7" t="n">
         <v>0.9684453780335274</v>
@@ -9247,10 +9247,10 @@
         <v>1.4206161862099087</v>
       </c>
       <c r="D8" t="n">
-        <v>15.226627750000002</v>
+        <v>12.885081249999997</v>
       </c>
       <c r="E8" t="n">
-        <v>1.5941053225000044</v>
+        <v>-0.7474411775000007</v>
       </c>
       <c r="F8" t="n">
         <v>0.8957921255024535</v>
@@ -9268,10 +9268,10 @@
         <v>0.922325000887472</v>
       </c>
       <c r="M8" t="n">
-        <v>158.97508123642908</v>
+        <v>158.95269213622393</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.4165636098426546</v>
+        <v>-0.43895271004780057</v>
       </c>
       <c r="O8" t="n">
         <v>0.9942134670749083</v>
@@ -9291,10 +9291,10 @@
         <v>0.8202229129198917</v>
       </c>
       <c r="D9" t="n">
-        <v>6.249899499999999</v>
+        <v>5.461013499999999</v>
       </c>
       <c r="E9" t="n">
-        <v>0.3719126924999996</v>
+        <v>-0.41697330750000017</v>
       </c>
       <c r="F9" t="n">
         <v>0.8604585311635387</v>
@@ -9312,10 +9312,10 @@
         <v>0.9997952083060258</v>
       </c>
       <c r="M9" t="n">
-        <v>87.64042093754689</v>
+        <v>88.95137547579543</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.5515844070551879</v>
+        <v>0.7593701311933501</v>
       </c>
       <c r="O9" t="n">
         <v>0.988663425846828</v>
@@ -9335,10 +9335,10 @@
         <v>4.438386934050192</v>
       </c>
       <c r="D10" t="n">
-        <v>45.03974074999999</v>
+        <v>41.630899</v>
       </c>
       <c r="E10" t="n">
-        <v>3.266254130000007</v>
+        <v>-0.14258761999998626</v>
       </c>
       <c r="F10" t="n">
         <v>0.8937511016395453</v>
@@ -9356,10 +9356,10 @@
         <v>1.0019416525493787</v>
       </c>
       <c r="M10" t="n">
-        <v>75.00178929657703</v>
+        <v>74.7849416793606</v>
       </c>
       <c r="N10" t="n">
-        <v>0.27854465147656526</v>
+        <v>0.06169703426013484</v>
       </c>
       <c r="O10" t="n">
         <v>0.9865912989015918</v>
@@ -9379,10 +9379,10 @@
         <v>2.5759863737446898</v>
       </c>
       <c r="D11" t="n">
-        <v>18.959232249999996</v>
+        <v>15.39517</v>
       </c>
       <c r="E11" t="n">
-        <v>1.9918035649999943</v>
+        <v>-1.5722586850000013</v>
       </c>
       <c r="F11" t="n">
         <v>0.8481805097538448</v>
@@ -9400,10 +9400,10 @@
         <v>0.6876061283844943</v>
       </c>
       <c r="M11" t="n">
-        <v>163.78093162494042</v>
+        <v>163.61691374741625</v>
       </c>
       <c r="N11" t="n">
-        <v>0.008858195877735398</v>
+        <v>-0.15515968164643823</v>
       </c>
       <c r="O11" t="n">
         <v>0.9958014445687389</v>
@@ -9423,10 +9423,10 @@
         <v>2.1308196229406713</v>
       </c>
       <c r="D12" t="n">
-        <v>4.0894685</v>
+        <v>4.101573000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.4761868424999971</v>
+        <v>-0.4640823424999958</v>
       </c>
       <c r="F12" t="n">
         <v>0.5332938071111808</v>
@@ -9444,10 +9444,10 @@
         <v>0.47496863635749725</v>
       </c>
       <c r="M12" t="n">
-        <v>26.648822360846676</v>
+        <v>26.104832130023166</v>
       </c>
       <c r="N12" t="n">
-        <v>0.41756160757423544</v>
+        <v>-0.12642862324927506</v>
       </c>
       <c r="O12" t="n">
         <v>0.9818930305780958</v>
@@ -9467,10 +9467,10 @@
         <v>2.0703441533791143</v>
       </c>
       <c r="D13" t="n">
-        <v>13.502141249999998</v>
+        <v>10.770157</v>
       </c>
       <c r="E13" t="n">
-        <v>1.318360969999997</v>
+        <v>-1.4136232800000013</v>
       </c>
       <c r="F13" t="n">
         <v>0.8300737451103218</v>
@@ -9488,10 +9488,10 @@
         <v>0.8497999538099986</v>
       </c>
       <c r="M13" t="n">
-        <v>153.46252723917135</v>
+        <v>155.04844673000753</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.7757422087534849</v>
+        <v>0.8101772820826909</v>
       </c>
       <c r="O13" t="n">
         <v>0.994490343046173</v>
@@ -9511,10 +9511,10 @@
         <v>2.351838495747105</v>
       </c>
       <c r="D14" t="n">
-        <v>22.4719305</v>
+        <v>18.460378249999998</v>
       </c>
       <c r="E14" t="n">
-        <v>2.6068666675000074</v>
+        <v>-1.4046855824999938</v>
       </c>
       <c r="F14" t="n">
         <v>0.8816093159540012</v>
@@ -9532,10 +9532,10 @@
         <v>0.793725850828756</v>
       </c>
       <c r="M14" t="n">
-        <v>161.93272048892686</v>
+        <v>160.64476524940255</v>
       </c>
       <c r="N14" t="n">
-        <v>0.46394988318041896</v>
+        <v>-0.8240053563438892</v>
       </c>
       <c r="O14" t="n">
         <v>0.9950843383036168</v>
@@ -9555,10 +9555,10 @@
         <v>17.516660901849498</v>
       </c>
       <c r="D15" t="n">
-        <v>222.27190900000002</v>
+        <v>221.77872175</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.1125181875000294</v>
+        <v>-0.6057054375000632</v>
       </c>
       <c r="F15" t="n">
         <v>0.9212325200852279</v>
@@ -9576,10 +9576,10 @@
         <v>5.893024041317602</v>
       </c>
       <c r="M15" t="n">
-        <v>1423.169335238417</v>
+        <v>1427.684640833981</v>
       </c>
       <c r="N15" t="n">
-        <v>4.63461978875398</v>
+        <v>9.14992538431784</v>
       </c>
       <c r="O15" t="n">
         <v>0.9958456962828368</v>
@@ -9632,10 +9632,10 @@
         <v>39</v>
       </c>
       <c r="B2" t="n">
-        <v>10.414186663923617</v>
+        <v>11.079120448419363</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07803939839340147</v>
+        <v>0.08833257681409007</v>
       </c>
       <c r="D2" t="s">
         <v>40</v>
@@ -9644,10 +9644,10 @@
         <v>39</v>
       </c>
       <c r="H2" t="n">
-        <v>37.49107199012502</v>
+        <v>39.88483361430971</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2809418342162453</v>
+        <v>0.31799727653072424</v>
       </c>
       <c r="J2" t="s">
         <v>41</v>
@@ -9658,10 +9658,10 @@
         <v>42</v>
       </c>
       <c r="B3" t="n">
-        <v>10.405375085739303</v>
+        <v>4.091749876542871</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6556751020613024</v>
+        <v>0.10045046839319675</v>
       </c>
       <c r="D3" t="s">
         <v>40</v>
@@ -9670,10 +9670,10 @@
         <v>42</v>
       </c>
       <c r="H3" t="n">
-        <v>37.45935030866149</v>
+        <v>14.730299555554337</v>
       </c>
       <c r="I3" t="n">
-        <v>2.3604303674206886</v>
+        <v>0.36162168621550833</v>
       </c>
       <c r="J3" t="s">
         <v>41</v>
@@ -9684,10 +9684,10 @@
         <v>43</v>
       </c>
       <c r="B4" t="n">
-        <v>10.655960989090408</v>
+        <v>11.607927359373278</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1272605155492091</v>
+        <v>0.14554312498087568</v>
       </c>
       <c r="D4" t="s">
         <v>40</v>
@@ -9696,10 +9696,10 @@
         <v>43</v>
       </c>
       <c r="H4" t="n">
-        <v>38.36145956072547</v>
+        <v>41.7885384937438</v>
       </c>
       <c r="I4" t="n">
-        <v>0.45813785597715284</v>
+        <v>0.5239552499311525</v>
       </c>
       <c r="J4" t="s">
         <v>41</v>
@@ -9710,10 +9710,10 @@
         <v>44</v>
       </c>
       <c r="B5" t="n">
-        <v>9.812493371696634</v>
+        <v>10.620070838362635</v>
       </c>
       <c r="C5" t="n">
-        <v>1.1893968345811738</v>
+        <v>1.3974906086895729</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -9722,10 +9722,10 @@
         <v>44</v>
       </c>
       <c r="H5" t="n">
-        <v>35.324976138107886</v>
+        <v>38.232255018105484</v>
       </c>
       <c r="I5" t="n">
-        <v>4.281828604492226</v>
+        <v>5.030966191282462</v>
       </c>
       <c r="J5" t="s">
         <v>41</v>
@@ -9736,10 +9736,10 @@
         <v>45</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8142124743713647</v>
+        <v>0.7120539642743513</v>
       </c>
       <c r="C6" t="n">
-        <v>0.030212199628910322</v>
+        <v>0.023556205107802024</v>
       </c>
       <c r="D6" t="s">
         <v>40</v>
@@ -9748,10 +9748,10 @@
         <v>45</v>
       </c>
       <c r="H6" t="n">
-        <v>2.931164907736913</v>
+        <v>2.563394271387665</v>
       </c>
       <c r="I6" t="n">
-        <v>0.10876391866407716</v>
+        <v>0.08480233838808729</v>
       </c>
       <c r="J6" t="s">
         <v>41</v>
@@ -9762,10 +9762,10 @@
         <v>46</v>
       </c>
       <c r="B7" t="n">
-        <v>8.61877154100583</v>
+        <v>8.724860630048484</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0605639651641692</v>
+        <v>0.06347725813862823</v>
       </c>
       <c r="D7" t="s">
         <v>40</v>
@@ -9774,10 +9774,10 @@
         <v>46</v>
       </c>
       <c r="H7" t="n">
-        <v>31.027577547620986</v>
+        <v>31.409498268174545</v>
       </c>
       <c r="I7" t="n">
-        <v>0.21803027459100913</v>
+        <v>0.22851812929906162</v>
       </c>
       <c r="J7" t="s">
         <v>41</v>
@@ -9788,10 +9788,10 @@
         <v>47</v>
       </c>
       <c r="B8" t="n">
-        <v>10.440596818059669</v>
+        <v>12.336180816572186</v>
       </c>
       <c r="C8" t="n">
-        <v>0.09759698963529764</v>
+        <v>0.1361980698348556</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
@@ -9800,10 +9800,10 @@
         <v>47</v>
       </c>
       <c r="H8" t="n">
-        <v>37.58614854501481</v>
+        <v>44.410250939659875</v>
       </c>
       <c r="I8" t="n">
-        <v>0.3513491626870715</v>
+        <v>0.4903130514054802</v>
       </c>
       <c r="J8" t="s">
         <v>41</v>
@@ -9814,10 +9814,10 @@
         <v>48</v>
       </c>
       <c r="B9" t="n">
-        <v>14.022692834908291</v>
+        <v>16.288437205986664</v>
       </c>
       <c r="C9" t="n">
-        <v>0.18472466781855088</v>
+        <v>0.24533003970386885</v>
       </c>
       <c r="D9" t="s">
         <v>40</v>
@@ -9826,10 +9826,10 @@
         <v>48</v>
       </c>
       <c r="H9" t="n">
-        <v>50.48169420566985</v>
+        <v>58.63837394155199</v>
       </c>
       <c r="I9" t="n">
-        <v>0.6650088041467832</v>
+        <v>0.8831881429339279</v>
       </c>
       <c r="J9" t="s">
         <v>41</v>
@@ -9840,10 +9840,10 @@
         <v>49</v>
       </c>
       <c r="B10" t="n">
-        <v>1.6652358128099802</v>
+        <v>1.7963806565733929</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01655996400472885</v>
+        <v>0.019302347978012876</v>
       </c>
       <c r="D10" t="s">
         <v>40</v>
@@ -9852,10 +9852,10 @@
         <v>49</v>
       </c>
       <c r="H10" t="n">
-        <v>5.994848926115929</v>
+        <v>6.466970363664214</v>
       </c>
       <c r="I10" t="n">
-        <v>0.05961587041702386</v>
+        <v>0.06948845272084636</v>
       </c>
       <c r="J10" t="s">
         <v>41</v>
@@ -9866,10 +9866,10 @@
         <v>50</v>
       </c>
       <c r="B11" t="n">
-        <v>8.638584593790208</v>
+        <v>10.627808185776205</v>
       </c>
       <c r="C11" t="n">
-        <v>0.11742826275302161</v>
+        <v>0.17788515947154618</v>
       </c>
       <c r="D11" t="s">
         <v>40</v>
@@ -9878,10 +9878,10 @@
         <v>50</v>
       </c>
       <c r="H11" t="n">
-        <v>31.09890453764475</v>
+        <v>38.26010946879434</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4227417459108778</v>
+        <v>0.6403865740975663</v>
       </c>
       <c r="J11" t="s">
         <v>41</v>
@@ -9892,10 +9892,10 @@
         <v>51</v>
       </c>
       <c r="B12" t="n">
-        <v>6.51645130922189</v>
+        <v>6.3645903973970865</v>
       </c>
       <c r="C12" t="n">
-        <v>0.33973860967753566</v>
+        <v>0.3308513311523656</v>
       </c>
       <c r="D12" t="s">
         <v>40</v>
@@ -9904,10 +9904,10 @@
         <v>51</v>
       </c>
       <c r="H12" t="n">
-        <v>23.459224713198804</v>
+        <v>22.91252543062951</v>
       </c>
       <c r="I12" t="n">
-        <v>1.2230589948391284</v>
+        <v>1.1910647921485162</v>
       </c>
       <c r="J12" t="s">
         <v>41</v>
@@ -9918,10 +9918,10 @@
         <v>52</v>
       </c>
       <c r="B13" t="n">
-        <v>11.365791869431924</v>
+        <v>14.396117598843501</v>
       </c>
       <c r="C13" t="n">
-        <v>0.17439041783941456</v>
+        <v>0.2768486125091275</v>
       </c>
       <c r="D13" t="s">
         <v>40</v>
@@ -9930,10 +9930,10 @@
         <v>52</v>
       </c>
       <c r="H13" t="n">
-        <v>40.91685072995492</v>
+        <v>51.826023355836604</v>
       </c>
       <c r="I13" t="n">
-        <v>0.6278055042218924</v>
+        <v>0.9966550050328591</v>
       </c>
       <c r="J13" t="s">
         <v>41</v>
@@ -9944,10 +9944,10 @@
         <v>53</v>
       </c>
       <c r="B14" t="n">
-        <v>7.205999524114177</v>
+        <v>8.70213833508003</v>
       </c>
       <c r="C14" t="n">
-        <v>0.07549829286370431</v>
+        <v>0.11094794078322623</v>
       </c>
       <c r="D14" t="s">
         <v>40</v>
@@ -9956,10 +9956,10 @@
         <v>53</v>
       </c>
       <c r="H14" t="n">
-        <v>25.94159828681104</v>
+        <v>31.327698006288106</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2717938543093355</v>
+        <v>0.39941258681961445</v>
       </c>
       <c r="J14" t="s">
         <v>41</v>
@@ -9970,10 +9970,10 @@
         <v>54</v>
       </c>
       <c r="B15" t="n">
-        <v>6.402830396523102</v>
+        <v>6.437428395152074</v>
       </c>
       <c r="C15" t="n">
-        <v>0.050528616619386534</v>
+        <v>0.05091387077458165</v>
       </c>
       <c r="D15" t="s">
         <v>40</v>
@@ -9982,10 +9982,10 @@
         <v>54</v>
       </c>
       <c r="H15" t="n">
-        <v>23.05018942748317</v>
+        <v>23.17474222254747</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1819030198297915</v>
+        <v>0.18328993478849395</v>
       </c>
       <c r="J15" t="s">
         <v>41</v>

</xml_diff>